<commit_message>
updated supplies model to Items and updated serverjs file to sync the database upon server start
</commit_message>
<xml_diff>
--- a/server/db/supplies_book_1.xlsx
+++ b/server/db/supplies_book_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manager\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorvil/Desktop/STEVEN(hard drive)/EDUCATION/CUNY SPS - BS Information Systems/2023 FALL/IS 499/classwork/staples-supply-management/server/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0BD9725-6739-489F-8C6F-D9DE4A52417B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E895D1-BFDA-6742-8B31-2D14DD194BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17205" yWindow="4785" windowWidth="21600" windowHeight="11385" xr2:uid="{19EE4B8A-1A9E-42DD-BAFB-81936C1DA736}"/>
+    <workbookView xWindow="16800" yWindow="4780" windowWidth="21600" windowHeight="16160" xr2:uid="{19EE4B8A-1A9E-42DD-BAFB-81936C1DA736}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="224">
   <si>
     <t>SKU</t>
   </si>
@@ -84,222 +84,21 @@
     <t xml:space="preserve">AIRTAG PRICE/PULL CARD KIT    </t>
   </si>
   <si>
-    <t xml:space="preserve"> 009-047-437-437</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 009-047-435-435</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 009-047-441-441</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-2.25MIL-40X28-100/CS      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-2.25MIL-8X40-500/CS       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-M LARGE                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-M SMALL                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-NON WOVEN-50/CS           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-PAPER REGISTER-300/BALE   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-PLASTIC REGISTER-500/CS   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-PLASTIC MED REG-2000CS    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-RACKS(HOLDER) 2PK         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-RECYCLE-SMALL-75/CS       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-RECYCLE-LARGE-75/CS       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BAG-REFILL FOR HP RETRIEVAL UN</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 009-047-442-442</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CREW BOTTLE &amp; TRIGGER         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CREW NA CLEANER-1 BTL         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CREW NA CLEANER-32OZ EA       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CROSSBAR ARM/CLIP PROMO-10/BX </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CROSSBAR-4FTX2IN-2PK          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CROSSBAR-1/2INX4FT-FLAT-4/BOX </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CROSSBAR KIT FOR COLLABORATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CROSSBAR-36X1/2-2/BOX         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CROSSBAR-36X2-2/BOX           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CROSSBAR-36X5-2/BOX           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CROSSBAR-36X11-2/BOX          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CROSSBAR-48X1/2-2/BOX         </t>
-  </si>
-  <si>
     <t>009-047-435-435</t>
   </si>
   <si>
     <t>009-047-437-437</t>
   </si>
   <si>
-    <t xml:space="preserve"> DISP ASTM LEV 3 MASK-50PK     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISP BUS HOURS OYSTER         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISP-BUSINESS HOURS-SS        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISPENSER-AIR FRESHENER       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISPENSER-BUBBLE WRAP 12IN PRF</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISPENSER-GP TOILET TISSUE    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISPENSER-KC ROLL TOWEL       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISPENSER-KC TOILET TISSUE    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISPENSER - SOAP              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISPENSER-TOILET SEAT         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISPENSER-W/PEANUTS LOOSE FILL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DISP FIX POSTER SGN STAND     </t>
-  </si>
-  <si>
     <t>009-047-450-450</t>
   </si>
   <si>
-    <t xml:space="preserve"> EASY REBATE DEMO              </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EASY TECH 2.0 PRODUCTION BOARD</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EASY TECH SIG MOMENT FOLDER-25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EASY TECH TABLET APP-10PK     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EASY TECH TEAR PAD-5/PK       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> E2G PRICE CHANNEL DISPLAY     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EMPTY BOX                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EMPTY BOX-ARLO1080 HD SEC CAM </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EMPTYBOX-ARLO VMC3040S SECCAM </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EMPTY BOX-ARLO SILICONE SKIN  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EMPTY BOX-ARLO SMART HOME CAM </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EMPTY BOX-ARLO HD 1 CAMERA KIT</t>
-  </si>
-  <si>
     <t>009-047-438-438</t>
   </si>
   <si>
     <t>009-047-444-444</t>
   </si>
   <si>
-    <t xml:space="preserve"> FIRST-AID TRIANGULAR BANDAGE  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIX-ADHESIVE VENDOR TAG-25/CS </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXT-5 PACK BINDER VIGNETTE   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXTUER-OXO SPINNER           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXTURE-BASE DECK SIGN CHANNEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXTURE-BBSLIDE DIVIDER GRAY  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXTURE-BBSLIDE DIVIDER OYSTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXTURE - DIGITAL VOICE       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXTURE-GIFT CARD TOWER       </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXTURE - OXO ISLAND DISPLAY  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXTURE-OXO ENDCAP KIT        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FIXTURE-OXO GLORIFIER         </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GRAY TEE SHIRT-4XL-DMA STORES</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GRAY TEE SHIRT-2XL-DMA STORES</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GRAY TEE SHIRT-3XL-DMA STORES</t>
-  </si>
-  <si>
     <t xml:space="preserve">GRAY UNISEX TEE-6XL-W&amp;L </t>
   </si>
   <si>
@@ -624,42 +423,6 @@
     <t xml:space="preserve">TAX 20 DOVER SIGN KIT 7       </t>
   </si>
   <si>
-    <t xml:space="preserve"> UNISEX RED TEE-2XL-S/S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX RED TEE-3XL-S/S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX RED TEE-4XL-S/S</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX TEE-LG SS      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX TEE-MED SS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX TEE-SM SS      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX TEE-4XL SS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX TEE-2XL SS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX TEE-3XL SS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX TEE-XL SS      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNISEX TEE-5XL SS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UNIV DIVIDER ARMS-3PK </t>
-  </si>
-  <si>
     <t xml:space="preserve">VACUUM BAGS-ROYAL-10PK     </t>
   </si>
   <si>
@@ -718,6 +481,231 @@
   </si>
   <si>
     <t>ZIP TIES FOR RTW TOTES-100/BAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-2.25MIL-40X28-100/CS      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-2.25MIL-8X40-500/CS       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-M LARGE                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-M SMALL                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-NON WOVEN-50/CS           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-PAPER REGISTER-300/BALE   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-PLASTIC REGISTER-500/CS   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-PLASTIC MED REG-2000CS    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-RACKS(HOLDER) 2PK         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-RECYCLE-SMALL-75/CS       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-RECYCLE-LARGE-75/CS       </t>
+  </si>
+  <si>
+    <t>BAG-REFILL FOR HP RETRIEVAL UN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREW BOTTLE &amp; TRIGGER         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREW NACLEANER-1 BTL         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREW NACLEANER-32OZ EA       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR ARM/CLIP PROMO-10/BX </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR-4FTX2IN-2PK          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR-1/2INX4FT-FLAT-4/BOX </t>
+  </si>
+  <si>
+    <t>CROSSBAR KIT FORCOLLABORATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR-36X1/2-2/BOX         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR-36X2-2/BOX           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR-36X5-2/BOX           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR-36X11-2/BOX          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR-48X1/2-2/BOX         </t>
+  </si>
+  <si>
+    <t>UNISEX RED TEE-2XL-S/S</t>
+  </si>
+  <si>
+    <t>UNISEX RED TEE-3XL-S/S</t>
+  </si>
+  <si>
+    <t>UNISEX RED TEE-4XL-S/S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-LG SS      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-MED SS     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-SM SS      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-4XL SS     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-2XL SS     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-3XL SS     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-XL SS      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-5XL SS     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIV DIVIDER ARMS-3PK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISP ASTM LEV 3 MASK-50PK     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISP BUS HOURS OYSTER         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISP-BUSINESS HOURS-SS        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER-AIR FRESHENER       </t>
+  </si>
+  <si>
+    <t>DISPENSER-BUBBLE WRAP 12IN PRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER-GP TOILET TISSUE    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER-KC ROLL TOWEL       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER-KC TOILET TISSUE    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER - SOAP              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER-TOILET SEAT         </t>
+  </si>
+  <si>
+    <t>DISPENSER-W/PEANUTS LOOSE FILL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISP FIX POSTER SGN STAND     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EASY REBATE DEMO              </t>
+  </si>
+  <si>
+    <t>EASY TECH 2.0 PRODUCTION BOARD</t>
+  </si>
+  <si>
+    <t>EASY TECH SIG MOMENT FOLDER-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EASY TECH TABLET APP-10PK     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EASY TECH TEAR PAD-5/PK       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2G PRICE CHANNEL DISPLAY     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMPTY BOX                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMPTY BOX-ARLO1080 HD SEC CAM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMPTYBOX-ARLO VMC3040S SECCAM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMPTY BOX-ARLO SILICONE SKIN  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMPTY BOX-ARLO SMART HOME CAM </t>
+  </si>
+  <si>
+    <t>EMPTY BOX-ARLO HD 1 CAMERA KIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXTURE-OXO ENDCAP KIT        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXTURE-OXO GLORIFIER         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRST-AID TRIANGULAR BANDAGE  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIX-ADHESIVE VENDOR TAG-25/CS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXT-5 PACK BINDER VIGNETTE   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXTUER-OXO SPINNER           </t>
+  </si>
+  <si>
+    <t>FIXTURE-BASE DECK SIGN CHANNEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXTURE-BBSLIDE DIVIDER GRAY  </t>
+  </si>
+  <si>
+    <t>FIXTURE-BBSLIDE DIVIDER OYSTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXTURE - DIGITAL VOICE       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXTURE-GIFT CARD TOWER       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXTURE - OXO ISLAND DISPLAY  </t>
+  </si>
+  <si>
+    <t>GRAY TEE SHIRT-4XL-DMA STORES</t>
+  </si>
+  <si>
+    <t>GRAY TEE SHIRT-2XL-DMA STORES</t>
+  </si>
+  <si>
+    <t>GRAY TEE SHIRT-3XL-DMA STORES</t>
   </si>
 </sst>
 </file>
@@ -1086,19 +1074,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E6C943-6578-48F5-97FE-52C0E228B8D4}">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D204" sqref="D204:D206"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2636750</v>
       </c>
@@ -1123,10 +1111,10 @@
         <v>0.01</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2636751</v>
       </c>
@@ -1137,10 +1125,10 @@
         <v>0.01</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>861198</v>
       </c>
@@ -1151,10 +1139,10 @@
         <v>0.01</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>680462</v>
       </c>
@@ -1165,10 +1153,10 @@
         <v>4.5</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>581080</v>
       </c>
@@ -1179,10 +1167,10 @@
         <v>26.16</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>721047</v>
       </c>
@@ -1193,10 +1181,10 @@
         <v>31.95</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>797995</v>
       </c>
@@ -1207,10 +1195,10 @@
         <v>0.01</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2554453</v>
       </c>
@@ -1221,10 +1209,10 @@
         <v>0.01</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1944628</v>
       </c>
@@ -1235,10 +1223,10 @@
         <v>0.01</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>24375279</v>
       </c>
@@ -1249,10 +1237,10 @@
         <v>0.01</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>24462109</v>
       </c>
@@ -1263,10 +1251,10 @@
         <v>0.01</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>24507841</v>
       </c>
@@ -1277,2709 +1265,2709 @@
         <v>0.01</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>120565</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="C14">
         <v>39.5</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>120566</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="C15">
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>753865</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="C16">
         <v>0.01</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>753864</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>152</v>
       </c>
       <c r="C17">
         <v>0.01</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2103529</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>153</v>
       </c>
       <c r="C18">
         <v>0.01</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>830474</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>154</v>
       </c>
       <c r="C19">
         <v>46.55</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>820222</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="C20">
         <v>49.29</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>24486274</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>156</v>
       </c>
       <c r="C21">
         <v>43.45</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>489906</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="C22">
         <v>59.16</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>698387</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>158</v>
       </c>
       <c r="C23">
         <v>14.54</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>698389</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
       <c r="C24">
         <v>35.21</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>387288</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="C25">
         <v>0.01</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>375782</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>161</v>
       </c>
       <c r="C26">
         <v>0.37</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>477808</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="C27">
         <v>23.75</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>24441152</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>163</v>
       </c>
       <c r="C28">
         <v>1.56</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>122718</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>164</v>
       </c>
       <c r="C29">
         <v>29.55</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>24399258</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>165</v>
       </c>
       <c r="C30">
         <v>0.01</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1921941</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="C31">
         <v>0.01</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>24522078</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>167</v>
       </c>
       <c r="C32">
         <v>0.01</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1924772</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>168</v>
       </c>
       <c r="C33">
         <v>0.01</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1924773</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="C34">
         <v>0.01</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1924774</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>170</v>
       </c>
       <c r="C35">
         <v>0.01</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1924775</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>171</v>
       </c>
       <c r="C36">
         <v>0.01</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1924776</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>172</v>
       </c>
       <c r="C37">
         <v>0.01</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>24520258</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>185</v>
       </c>
       <c r="C38">
         <v>5.5</v>
       </c>
       <c r="D38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>399890</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>186</v>
       </c>
       <c r="C39">
         <v>0.01</v>
       </c>
       <c r="D39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>399198</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>187</v>
       </c>
       <c r="C40">
         <v>0.01</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>674158</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>188</v>
       </c>
       <c r="C41">
         <v>28</v>
       </c>
       <c r="D41" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>396538</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>189</v>
       </c>
       <c r="C42">
         <v>17.75</v>
       </c>
       <c r="D42" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>385169</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>190</v>
       </c>
       <c r="C43">
         <v>0.01</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>918748</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>191</v>
       </c>
       <c r="C44">
         <v>0.01</v>
       </c>
       <c r="D44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2758595</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>192</v>
       </c>
       <c r="C45">
         <v>0.01</v>
       </c>
       <c r="D45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>919623</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="C46">
         <v>0.01</v>
       </c>
       <c r="D46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>385163</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>194</v>
       </c>
       <c r="C47">
         <v>5.13</v>
       </c>
       <c r="D47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>396540</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>195</v>
       </c>
       <c r="C48">
         <v>11.69</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2843067</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>196</v>
       </c>
       <c r="C49">
         <v>0.01</v>
       </c>
       <c r="D49" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>746309</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>197</v>
       </c>
       <c r="C50">
         <v>0.01</v>
       </c>
       <c r="D50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>902635</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>198</v>
       </c>
       <c r="C51">
         <v>198.48</v>
       </c>
       <c r="D51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>798378</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>199</v>
       </c>
       <c r="C52">
         <v>22.05</v>
       </c>
       <c r="D52" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>163433</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>200</v>
       </c>
       <c r="C53">
         <v>0.01</v>
       </c>
       <c r="D53" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>358954</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>201</v>
       </c>
       <c r="C54">
         <v>6.33</v>
       </c>
       <c r="D54" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>130442</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>202</v>
       </c>
       <c r="C55">
         <v>0.01</v>
       </c>
       <c r="D55" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1571565</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>203</v>
       </c>
       <c r="C56">
         <v>0.01</v>
       </c>
       <c r="D56" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>24401194</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>204</v>
       </c>
       <c r="C57">
         <v>0.01</v>
       </c>
       <c r="D57" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>24401195</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>205</v>
       </c>
       <c r="C58">
         <v>0.01</v>
       </c>
       <c r="D58" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>24401196</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>206</v>
       </c>
       <c r="C59">
         <v>0.01</v>
       </c>
       <c r="D59" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>24401197</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>207</v>
       </c>
       <c r="C60">
         <v>0.01</v>
       </c>
       <c r="D60" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>24401198</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>208</v>
       </c>
       <c r="C61">
         <v>0.01</v>
       </c>
       <c r="D61" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>485797</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>211</v>
       </c>
       <c r="C62">
         <v>0.49</v>
       </c>
       <c r="D62" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>668364</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>212</v>
       </c>
       <c r="C63">
         <v>62.5</v>
       </c>
       <c r="D63" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>737795</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>213</v>
       </c>
       <c r="C64">
         <v>0.01</v>
       </c>
       <c r="D64" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>791654</v>
       </c>
       <c r="B65" t="s">
-        <v>76</v>
+        <v>214</v>
       </c>
       <c r="C65">
         <v>0.01</v>
       </c>
       <c r="D65" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>821806</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>215</v>
       </c>
       <c r="C66">
         <v>0.01</v>
       </c>
       <c r="D66" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>797525</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>216</v>
       </c>
       <c r="C67">
         <v>0.01</v>
       </c>
       <c r="D67" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>797527</v>
       </c>
       <c r="B68" t="s">
-        <v>79</v>
+        <v>217</v>
       </c>
       <c r="C68">
         <v>0.01</v>
       </c>
       <c r="D68" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>791718</v>
       </c>
       <c r="B69" t="s">
-        <v>80</v>
+        <v>218</v>
       </c>
       <c r="C69">
         <v>0.01</v>
       </c>
       <c r="D69" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>764677</v>
       </c>
       <c r="B70" t="s">
-        <v>81</v>
+        <v>219</v>
       </c>
       <c r="C70">
         <v>0.01</v>
       </c>
       <c r="D70" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>781812</v>
       </c>
       <c r="B71" t="s">
-        <v>82</v>
+        <v>220</v>
       </c>
       <c r="C71">
         <v>0.01</v>
       </c>
       <c r="D71" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>791655</v>
       </c>
       <c r="B72" t="s">
-        <v>83</v>
+        <v>209</v>
       </c>
       <c r="C72">
         <v>0.01</v>
       </c>
       <c r="D72" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>814168</v>
       </c>
       <c r="B73" t="s">
-        <v>84</v>
+        <v>210</v>
       </c>
       <c r="C73">
         <v>0.01</v>
       </c>
       <c r="D73" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>24430271</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>221</v>
       </c>
       <c r="C74">
         <v>0.01</v>
       </c>
       <c r="D74" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>24430272</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
+        <v>222</v>
       </c>
       <c r="C75">
         <v>0.01</v>
       </c>
       <c r="D75" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>24430273</v>
       </c>
       <c r="B76" t="s">
-        <v>87</v>
+        <v>223</v>
       </c>
       <c r="C76">
         <v>0.01</v>
       </c>
       <c r="D76" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>24430274</v>
       </c>
       <c r="B77" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="C77">
         <v>0.01</v>
       </c>
       <c r="D77" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>24430275</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="C78">
         <v>0.01</v>
       </c>
       <c r="D78" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>24479433</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="C79">
         <v>0.01</v>
       </c>
       <c r="D79" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>24443470</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="C80">
         <v>97.37</v>
       </c>
       <c r="D80" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>24449149</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="C81">
         <v>23</v>
       </c>
       <c r="D81" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1056170</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="C82">
         <v>0.01</v>
       </c>
       <c r="D82" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>749931</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="C83">
         <v>0.01</v>
       </c>
       <c r="D83" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>24547928</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="C84">
         <v>0.01</v>
       </c>
       <c r="D84" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2115890</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="C85">
         <v>0.01</v>
       </c>
       <c r="D85" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>24500475</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="C86">
         <v>0.01</v>
       </c>
       <c r="D86" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>930831</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="C87">
         <v>0.01</v>
       </c>
       <c r="D87" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2112627</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="C88">
         <v>0.01</v>
       </c>
       <c r="D88" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>761485</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="C89">
         <v>1.4</v>
       </c>
       <c r="D89" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>24539938</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="C90">
         <v>0.01</v>
       </c>
       <c r="D90" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>24421441</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="C91">
         <v>0.01</v>
       </c>
       <c r="D91" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>571594</v>
       </c>
       <c r="B92" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="C92">
         <v>99</v>
       </c>
       <c r="D92" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>24473027</v>
       </c>
       <c r="B93" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="C93">
         <v>13.34</v>
       </c>
       <c r="D93" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>24473028</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="C94">
         <v>12.32</v>
       </c>
       <c r="D94" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>24473029</v>
       </c>
       <c r="B95" t="s">
-        <v>109</v>
+        <v>42</v>
       </c>
       <c r="C95">
         <v>13.35</v>
       </c>
       <c r="D95" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>24473030</v>
       </c>
       <c r="B96" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="C96">
         <v>13.23</v>
       </c>
       <c r="D96" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>674505</v>
       </c>
       <c r="B97" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="C97">
         <v>5.75</v>
       </c>
       <c r="D97" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>697353</v>
       </c>
       <c r="B98" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="C98">
         <v>6.57</v>
       </c>
       <c r="D98" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>439837</v>
       </c>
       <c r="B99" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="C99">
         <v>4.8600000000000003</v>
       </c>
       <c r="D99" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>382583</v>
       </c>
       <c r="B100" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="C100">
         <v>18.66</v>
       </c>
       <c r="D100" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>492754</v>
       </c>
       <c r="B101" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
       <c r="C101">
         <v>4.8499999999999996</v>
       </c>
       <c r="D101" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>747916</v>
       </c>
       <c r="B102" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="C102">
         <v>10.85</v>
       </c>
       <c r="D102" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>24581460</v>
       </c>
       <c r="B103" t="s">
-        <v>117</v>
+        <v>50</v>
       </c>
       <c r="C103">
         <v>0.01</v>
       </c>
       <c r="D103" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>868617</v>
       </c>
       <c r="B104" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="C104">
         <v>13.76</v>
       </c>
       <c r="D104" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>868618</v>
       </c>
       <c r="B105" t="s">
-        <v>120</v>
+        <v>53</v>
       </c>
       <c r="C105">
         <v>13.76</v>
       </c>
       <c r="D105" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>868619</v>
       </c>
       <c r="B106" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="C106">
         <v>13.77</v>
       </c>
       <c r="D106" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>868621</v>
       </c>
       <c r="B107" t="s">
-        <v>122</v>
+        <v>55</v>
       </c>
       <c r="C107">
         <v>13.76</v>
       </c>
       <c r="D107" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>868622</v>
       </c>
       <c r="B108" t="s">
-        <v>123</v>
+        <v>56</v>
       </c>
       <c r="C108">
         <v>14.73</v>
       </c>
       <c r="D108" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>868623</v>
       </c>
       <c r="B109" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="C109">
         <v>13.76</v>
       </c>
       <c r="D109" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>868656</v>
       </c>
       <c r="B110" t="s">
-        <v>125</v>
+        <v>58</v>
       </c>
       <c r="C110">
         <v>10.1</v>
       </c>
       <c r="D110" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>24374440</v>
       </c>
       <c r="B111" t="s">
-        <v>126</v>
+        <v>59</v>
       </c>
       <c r="C111">
         <v>13.76</v>
       </c>
       <c r="D111" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>24374441</v>
       </c>
       <c r="B112" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="C112">
         <v>13.96</v>
       </c>
       <c r="D112" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>24374442</v>
       </c>
       <c r="B113" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="C113">
         <v>13.76</v>
       </c>
       <c r="D113" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>24374443</v>
       </c>
       <c r="B114" t="s">
-        <v>129</v>
+        <v>62</v>
       </c>
       <c r="C114">
         <v>13.76</v>
       </c>
       <c r="D114" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>24374444</v>
       </c>
       <c r="B115" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="C115">
         <v>13.76</v>
       </c>
       <c r="D115" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>404427</v>
       </c>
       <c r="B116" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="C116">
         <v>0.01</v>
       </c>
       <c r="D116" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>307201</v>
       </c>
       <c r="B117" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="C117">
         <v>0.01</v>
       </c>
       <c r="D117" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2126719</v>
       </c>
       <c r="B118" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="C118">
         <v>0.01</v>
       </c>
       <c r="D118" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>24375375</v>
       </c>
       <c r="B119" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
       <c r="C119">
         <v>0.01</v>
       </c>
       <c r="D119" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>271715</v>
       </c>
       <c r="B120" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="C120">
         <v>0.01</v>
       </c>
       <c r="D120" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>24567572</v>
       </c>
       <c r="B121" t="s">
-        <v>136</v>
+        <v>69</v>
       </c>
       <c r="C121">
         <v>0.01</v>
       </c>
       <c r="D121" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>24387510</v>
       </c>
       <c r="B122" t="s">
-        <v>137</v>
+        <v>70</v>
       </c>
       <c r="C122">
         <v>0.01</v>
       </c>
       <c r="D122" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1230742</v>
       </c>
       <c r="B123" t="s">
-        <v>138</v>
+        <v>71</v>
       </c>
       <c r="C123">
         <v>0.01</v>
       </c>
       <c r="D123" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>24319699</v>
       </c>
       <c r="B124" t="s">
-        <v>139</v>
+        <v>72</v>
       </c>
       <c r="C124">
         <v>0.01</v>
       </c>
       <c r="D124" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>24373366</v>
       </c>
       <c r="B125" t="s">
-        <v>140</v>
+        <v>73</v>
       </c>
       <c r="C125">
         <v>0.01</v>
       </c>
       <c r="D125" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>24526646</v>
       </c>
       <c r="B126" t="s">
-        <v>141</v>
+        <v>74</v>
       </c>
       <c r="C126">
         <v>0.01</v>
       </c>
       <c r="D126" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>24401869</v>
       </c>
       <c r="B127" t="s">
-        <v>142</v>
+        <v>75</v>
       </c>
       <c r="C127">
         <v>0.01</v>
       </c>
       <c r="D127" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>24399270</v>
       </c>
       <c r="B128" t="s">
-        <v>144</v>
+        <v>77</v>
       </c>
       <c r="C128">
         <v>79.48</v>
       </c>
       <c r="D128" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>24399271</v>
       </c>
       <c r="B129" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="C129">
         <v>118.63</v>
       </c>
       <c r="D129" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>24399272</v>
       </c>
       <c r="B130" t="s">
-        <v>146</v>
+        <v>79</v>
       </c>
       <c r="C130">
         <v>118.76</v>
       </c>
       <c r="D130" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>24399275</v>
       </c>
       <c r="B131" t="s">
-        <v>147</v>
+        <v>80</v>
       </c>
       <c r="C131">
         <v>79.400000000000006</v>
       </c>
       <c r="D131" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>24503275</v>
       </c>
       <c r="B132" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="C132">
         <v>102.04</v>
       </c>
       <c r="D132" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>426227</v>
       </c>
       <c r="B133" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="C133">
         <v>15.8</v>
       </c>
       <c r="D133" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>810026</v>
       </c>
       <c r="B134" t="s">
-        <v>150</v>
+        <v>83</v>
       </c>
       <c r="C134">
         <v>7.97</v>
       </c>
       <c r="D134" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>810029</v>
       </c>
       <c r="B135" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="C135">
         <v>10.98</v>
       </c>
       <c r="D135" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>24507652</v>
       </c>
       <c r="B136" t="s">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="C136">
         <v>9.89</v>
       </c>
       <c r="D136" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>24522057</v>
       </c>
       <c r="B137" t="s">
-        <v>153</v>
+        <v>86</v>
       </c>
       <c r="C137">
         <v>750</v>
       </c>
       <c r="D137" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>24522747</v>
       </c>
       <c r="B138" t="s">
-        <v>154</v>
+        <v>87</v>
       </c>
       <c r="C138">
         <v>0.01</v>
       </c>
       <c r="D138" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>24525624</v>
       </c>
       <c r="B139" t="s">
-        <v>155</v>
+        <v>88</v>
       </c>
       <c r="C139">
         <v>12.84</v>
       </c>
       <c r="D139" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>24508926</v>
       </c>
       <c r="B140" t="s">
-        <v>157</v>
+        <v>90</v>
       </c>
       <c r="C140">
         <v>0.01</v>
       </c>
       <c r="D140" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>1437976</v>
       </c>
       <c r="B141" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="C141">
         <v>57.95</v>
       </c>
       <c r="D141" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>788568</v>
       </c>
       <c r="B142" t="s">
-        <v>159</v>
+        <v>92</v>
       </c>
       <c r="C142">
         <v>44.96</v>
       </c>
       <c r="D142" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>24296490</v>
       </c>
       <c r="B143" t="s">
-        <v>160</v>
+        <v>93</v>
       </c>
       <c r="C143">
         <v>0.01</v>
       </c>
       <c r="D143" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>750022</v>
       </c>
       <c r="B144" t="s">
-        <v>161</v>
+        <v>94</v>
       </c>
       <c r="C144">
         <v>0.01</v>
       </c>
       <c r="D144" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>459125</v>
       </c>
       <c r="B145" t="s">
-        <v>162</v>
+        <v>95</v>
       </c>
       <c r="C145">
         <v>8.52</v>
       </c>
       <c r="D145" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>816222</v>
       </c>
       <c r="B146" t="s">
-        <v>163</v>
+        <v>96</v>
       </c>
       <c r="C146">
         <v>8.52</v>
       </c>
       <c r="D146" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>749905</v>
       </c>
       <c r="B147" t="s">
-        <v>164</v>
+        <v>97</v>
       </c>
       <c r="C147">
         <v>0.01</v>
       </c>
       <c r="D147" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>2707926</v>
       </c>
       <c r="B148" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="C148">
         <v>87.53</v>
       </c>
       <c r="D148" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>580556</v>
       </c>
       <c r="B149" t="s">
-        <v>166</v>
+        <v>99</v>
       </c>
       <c r="C149">
         <v>1.06</v>
       </c>
       <c r="D149" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>918563</v>
       </c>
       <c r="B150" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="C150">
         <v>25.35</v>
       </c>
       <c r="D150" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>24441153</v>
       </c>
       <c r="B151" t="s">
-        <v>168</v>
+        <v>101</v>
       </c>
       <c r="C151">
         <v>41.08</v>
       </c>
       <c r="D151" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>24520544</v>
       </c>
       <c r="B152" t="s">
-        <v>171</v>
+        <v>104</v>
       </c>
       <c r="C152">
         <v>16.22</v>
       </c>
       <c r="D152" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>24522741</v>
       </c>
       <c r="B153" t="s">
-        <v>172</v>
+        <v>105</v>
       </c>
       <c r="C153">
         <v>29.06</v>
       </c>
       <c r="D153" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>24528564</v>
       </c>
       <c r="B154" t="s">
-        <v>173</v>
+        <v>106</v>
       </c>
       <c r="C154">
         <v>16.43</v>
       </c>
       <c r="D154" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>24531210</v>
       </c>
       <c r="B155" t="s">
-        <v>174</v>
+        <v>107</v>
       </c>
       <c r="C155">
         <v>17.09</v>
       </c>
       <c r="D155" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>24531655</v>
       </c>
       <c r="B156" t="s">
-        <v>175</v>
+        <v>108</v>
       </c>
       <c r="C156">
         <v>19.940000000000001</v>
       </c>
       <c r="D156" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>24533744</v>
       </c>
       <c r="B157" t="s">
-        <v>176</v>
+        <v>109</v>
       </c>
       <c r="C157">
         <v>17.100000000000001</v>
       </c>
       <c r="D157" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>427724</v>
       </c>
       <c r="B158" t="s">
-        <v>177</v>
+        <v>110</v>
       </c>
       <c r="C158">
         <v>0.01</v>
       </c>
       <c r="D158" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>1958186</v>
       </c>
       <c r="B159" t="s">
-        <v>178</v>
+        <v>111</v>
       </c>
       <c r="C159">
         <v>0.01</v>
       </c>
       <c r="D159" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>721049</v>
       </c>
       <c r="B160" t="s">
-        <v>179</v>
+        <v>112</v>
       </c>
       <c r="C160">
         <v>180.91</v>
       </c>
       <c r="D160" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>369636</v>
       </c>
       <c r="B161" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
       <c r="C161">
         <v>126.78</v>
       </c>
       <c r="D161" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>710729</v>
       </c>
       <c r="B162" t="s">
-        <v>181</v>
+        <v>114</v>
       </c>
       <c r="C162">
         <v>191.58</v>
       </c>
       <c r="D162" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>800330</v>
       </c>
       <c r="B163" t="s">
-        <v>182</v>
+        <v>115</v>
       </c>
       <c r="C163">
         <v>0.01</v>
       </c>
       <c r="D163" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>404270</v>
       </c>
       <c r="B164" t="s">
-        <v>184</v>
+        <v>117</v>
       </c>
       <c r="C164">
         <v>16.059999999999999</v>
       </c>
       <c r="D164" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>596695</v>
       </c>
       <c r="B165" t="s">
-        <v>185</v>
+        <v>118</v>
       </c>
       <c r="C165">
         <v>10.91</v>
       </c>
       <c r="D165" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>24338269</v>
       </c>
       <c r="B166" t="s">
-        <v>186</v>
+        <v>119</v>
       </c>
       <c r="C166">
         <v>46.94</v>
       </c>
       <c r="D166" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>561287</v>
       </c>
       <c r="B167" t="s">
-        <v>187</v>
+        <v>120</v>
       </c>
       <c r="C167">
         <v>5.1100000000000003</v>
       </c>
       <c r="D167" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>1923563</v>
       </c>
       <c r="B168" t="s">
-        <v>188</v>
+        <v>121</v>
       </c>
       <c r="C168">
         <v>0.01</v>
       </c>
       <c r="D168" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>1923562</v>
       </c>
       <c r="B169" t="s">
-        <v>189</v>
+        <v>122</v>
       </c>
       <c r="C169">
         <v>0.01</v>
       </c>
       <c r="D169" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>24556794</v>
       </c>
       <c r="B170" t="s">
-        <v>190</v>
+        <v>123</v>
       </c>
       <c r="C170">
         <v>0.01</v>
       </c>
       <c r="D170" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>24525623</v>
       </c>
       <c r="B171" t="s">
-        <v>191</v>
+        <v>124</v>
       </c>
       <c r="C171">
         <v>0.01</v>
       </c>
       <c r="D171" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>24421186</v>
       </c>
       <c r="B172" t="s">
-        <v>192</v>
+        <v>125</v>
       </c>
       <c r="C172">
         <v>0.01</v>
       </c>
       <c r="D172" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>24421187</v>
       </c>
       <c r="B173" t="s">
-        <v>193</v>
+        <v>126</v>
       </c>
       <c r="C173">
         <v>0.01</v>
       </c>
       <c r="D173" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>24421188</v>
       </c>
       <c r="B174" t="s">
-        <v>194</v>
+        <v>127</v>
       </c>
       <c r="C174">
         <v>0.01</v>
       </c>
       <c r="D174" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>24421189</v>
       </c>
       <c r="B175" t="s">
-        <v>195</v>
+        <v>128</v>
       </c>
       <c r="C175">
         <v>0.01</v>
       </c>
       <c r="D175" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>1238234</v>
       </c>
       <c r="B176" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="C176">
         <v>5.88</v>
       </c>
       <c r="D176" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>1238240</v>
       </c>
       <c r="B177" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="C177">
         <v>5.88</v>
       </c>
       <c r="D177" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>1238241</v>
       </c>
       <c r="B178" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="C178">
         <v>5.88</v>
       </c>
       <c r="D178" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>24479430</v>
       </c>
       <c r="B179" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="C179">
         <v>7.04</v>
       </c>
       <c r="D179" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>24479426</v>
       </c>
       <c r="B180" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="C180">
         <v>7.04</v>
       </c>
       <c r="D180" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>24479425</v>
       </c>
       <c r="B181" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="C181">
         <v>7.04</v>
       </c>
       <c r="D181" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>24479427</v>
       </c>
       <c r="B182" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="C182">
         <v>11.9</v>
       </c>
       <c r="D182" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>24479428</v>
       </c>
       <c r="B183" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="C183">
         <v>9.8000000000000007</v>
       </c>
       <c r="D183" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>24479429</v>
       </c>
       <c r="B184" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="C184">
         <v>10.09</v>
       </c>
       <c r="D184" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>24479431</v>
       </c>
       <c r="B185" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="C185">
         <v>7.04</v>
       </c>
       <c r="D185" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>24479432</v>
       </c>
       <c r="B186" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="C186">
         <v>11.9</v>
       </c>
       <c r="D186" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>24488138</v>
       </c>
       <c r="B187" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C187">
         <v>0.01</v>
       </c>
       <c r="D187" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>579883</v>
       </c>
       <c r="B188" t="s">
-        <v>208</v>
+        <v>129</v>
       </c>
       <c r="C188">
         <v>11.25</v>
       </c>
       <c r="D188" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>809083</v>
       </c>
       <c r="B189" t="s">
-        <v>209</v>
+        <v>130</v>
       </c>
       <c r="C189">
         <v>19.239999999999998</v>
       </c>
       <c r="D189" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>369644</v>
       </c>
       <c r="B190" t="s">
-        <v>210</v>
+        <v>131</v>
       </c>
       <c r="C190">
         <v>10.5</v>
       </c>
       <c r="D190" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>378328</v>
       </c>
       <c r="B191" t="s">
-        <v>211</v>
+        <v>132</v>
       </c>
       <c r="C191">
         <v>14.4</v>
       </c>
       <c r="D191" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>24507775</v>
       </c>
       <c r="B192" t="s">
-        <v>212</v>
+        <v>133</v>
       </c>
       <c r="C192">
         <v>28.8</v>
       </c>
       <c r="D192" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>620140</v>
       </c>
       <c r="B193" t="s">
-        <v>213</v>
+        <v>134</v>
       </c>
       <c r="C193">
         <v>147.38999999999999</v>
       </c>
       <c r="D193" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>24507774</v>
       </c>
       <c r="B194" t="s">
-        <v>214</v>
+        <v>135</v>
       </c>
       <c r="C194">
         <v>51.7</v>
       </c>
       <c r="D194" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>626677</v>
       </c>
       <c r="B195" t="s">
-        <v>215</v>
+        <v>136</v>
       </c>
       <c r="C195">
         <v>20.75</v>
       </c>
       <c r="D195" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>789437</v>
       </c>
       <c r="B196" t="s">
-        <v>216</v>
+        <v>137</v>
       </c>
       <c r="C196">
         <v>5.98</v>
       </c>
       <c r="D196" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>355534</v>
       </c>
       <c r="B197" t="s">
-        <v>217</v>
+        <v>138</v>
       </c>
       <c r="C197">
         <v>10.1</v>
       </c>
       <c r="D197" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>355535</v>
       </c>
       <c r="B198" t="s">
-        <v>218</v>
+        <v>139</v>
       </c>
       <c r="C198">
         <v>12.9</v>
       </c>
       <c r="D198" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>116457</v>
       </c>
       <c r="B199" t="s">
-        <v>219</v>
+        <v>140</v>
       </c>
       <c r="C199">
         <v>0.01</v>
       </c>
       <c r="D199" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>24449148</v>
       </c>
       <c r="B200" t="s">
-        <v>220</v>
+        <v>141</v>
       </c>
       <c r="C200">
         <v>3.5</v>
       </c>
       <c r="D200" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>395073</v>
       </c>
       <c r="B201" t="s">
-        <v>221</v>
+        <v>142</v>
       </c>
       <c r="C201">
         <v>62.5</v>
       </c>
       <c r="D201" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>2846332</v>
       </c>
       <c r="B202" t="s">
-        <v>222</v>
+        <v>143</v>
       </c>
       <c r="C202">
         <v>0.01</v>
       </c>
       <c r="D202" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>24307465</v>
       </c>
       <c r="B203" t="s">
-        <v>223</v>
+        <v>144</v>
       </c>
       <c r="C203">
         <v>0.01</v>
       </c>
       <c r="D203" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>1897666</v>
       </c>
       <c r="B204" t="s">
-        <v>225</v>
+        <v>146</v>
       </c>
       <c r="C204">
         <v>1.77</v>
       </c>
       <c r="D204" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>1897667</v>
       </c>
       <c r="B205" t="s">
-        <v>226</v>
+        <v>147</v>
       </c>
       <c r="C205">
         <v>0.4</v>
       </c>
       <c r="D205" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>732290</v>
       </c>
       <c r="B206" t="s">
-        <v>227</v>
+        <v>148</v>
       </c>
       <c r="C206">
         <v>6.08</v>
       </c>
       <c r="D206" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recommit, excel file has been converted to sql database using sequelize, model for supplies updated, routes to be created next, and make routes modular.
</commit_message>
<xml_diff>
--- a/server/db/supplies_book_1.xlsx
+++ b/server/db/supplies_book_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorvil/Desktop/STEVEN(hard drive)/EDUCATION/CUNY SPS - BS Information Systems/2023 FALL/IS 499/classwork/staples-supply-management/server/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E895D1-BFDA-6742-8B31-2D14DD194BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D205176C-A02E-7F49-8A4A-B155C0E57CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="4780" windowWidth="21600" windowHeight="16160" xr2:uid="{19EE4B8A-1A9E-42DD-BAFB-81936C1DA736}"/>
+    <workbookView xWindow="7200" yWindow="1840" windowWidth="21600" windowHeight="16160" xr2:uid="{19EE4B8A-1A9E-42DD-BAFB-81936C1DA736}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E6C943-6578-48F5-97FE-52C0E228B8D4}">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
created basic crud routes for the items database. Get all items, get single items, create new item, edit an item, and delete an item. All the routes handle basic error checking, and routes are using sku number as reference.
</commit_message>
<xml_diff>
--- a/server/db/supplies_book_1.xlsx
+++ b/server/db/supplies_book_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorvil/Desktop/STEVEN(hard drive)/EDUCATION/CUNY SPS - BS Information Systems/2023 FALL/IS 499/classwork/staples-supply-management/server/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D205176C-A02E-7F49-8A4A-B155C0E57CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B26527-186B-5743-BF04-B28423CFDF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1840" windowWidth="21600" windowHeight="16160" xr2:uid="{19EE4B8A-1A9E-42DD-BAFB-81936C1DA736}"/>
   </bookViews>
@@ -48,42 +48,18 @@
     <t>dpt-sub-cls-sub</t>
   </si>
   <si>
-    <t xml:space="preserve">ACADEMY ACRYLIC RACK          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACADEMY OIL RACK              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">744788 AC BOX                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACRYLIC-SMALL CALCULATOR TBD  </t>
-  </si>
-  <si>
     <t xml:space="preserve">ACRYLIC-2 TIER DISPLAY HOLDER </t>
   </si>
   <si>
     <t xml:space="preserve">ACRYLIC-4 TIER DISPLAY HOLDER </t>
   </si>
   <si>
-    <t xml:space="preserve">A2 DOUBLE FRONT END (2PANEL)  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIO DISPLAY MAT               </t>
-  </si>
-  <si>
     <t>AIR PILLOW BUBBLE-48X12-100/CS</t>
   </si>
   <si>
     <t xml:space="preserve">AIR POD EMPTY BOX KIT-POG 342 </t>
   </si>
   <si>
-    <t xml:space="preserve">AIRPODS AUDIO SQUARE          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIRTAG PRICE/PULL CARD KIT    </t>
-  </si>
-  <si>
     <t>009-047-435-435</t>
   </si>
   <si>
@@ -111,84 +87,33 @@
     <t>009-047-439-439</t>
   </si>
   <si>
-    <t xml:space="preserve">HAND SANITIZER-24/CS          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HAND SANITIZER-1 GAL-75% ALC  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HAND TRUCK                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HAND WRAP - DC USE ONLY       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">H22 DECO CALENDAR TRAY        </t>
-  </si>
-  <si>
     <t xml:space="preserve">HDMI TO DVI ADAPTER CABLE-BLK </t>
   </si>
   <si>
-    <t xml:space="preserve">HIGH-DEFINITION MEDIA PLAYER  </t>
-  </si>
-  <si>
     <t>HIGH VELOCITY DUMP BIN SHIPPER</t>
   </si>
   <si>
-    <t xml:space="preserve">HIGH WALL USB SIGNAGE KIT     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HINGE-ELMERS-2PK              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HO22ET5150 SIGN               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOL19 ACER                    </t>
-  </si>
-  <si>
     <t>009-047-441-441</t>
   </si>
   <si>
     <t>009-047-440-440</t>
   </si>
   <si>
-    <t xml:space="preserve">LABEL-MA PRICE CHECKER-12RLS  </t>
-  </si>
-  <si>
     <t>LABEL-MATTE 6UP-3X3 CIRC-100PK</t>
   </si>
   <si>
-    <t xml:space="preserve">LABEL-MATTE 4UP-5X3 OVAL-100  </t>
-  </si>
-  <si>
     <t>LABEL-MATTE24UP-1.5X1.5CIRC100</t>
   </si>
   <si>
     <t xml:space="preserve">LABEL-MATTE 10UP-3X2 OVAL-100 </t>
   </si>
   <si>
-    <t xml:space="preserve">LABEL-PC WRAP-EZ TECH-500/RL  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LABEL-RECYCLE-500/ROLL        </t>
-  </si>
-  <si>
     <t>LABEL-SPECIAL CLEARANCE-500/RL</t>
   </si>
   <si>
-    <t xml:space="preserve">LABEL-TECH RETURN 5X4-800/RL  </t>
-  </si>
-  <si>
     <t>LABEL-TECH RETURN 2.5X2-500/RL</t>
   </si>
   <si>
-    <t xml:space="preserve">LABEL-22UP-100/PK             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LABEL UPS A-CAE1-500RL        </t>
-  </si>
-  <si>
     <t>009-047-448-448</t>
   </si>
   <si>
@@ -216,9 +141,6 @@
     <t xml:space="preserve">MANAGER WMNS POLO-XS-LS </t>
   </si>
   <si>
-    <t xml:space="preserve">MANAGER WMNS POLO-S-LS  </t>
-  </si>
-  <si>
     <t>MANAGER WMNS POLO-5XL-LS</t>
   </si>
   <si>
@@ -228,42 +150,9 @@
     <t>MANAGER WMNS POLO-4XL-LS</t>
   </si>
   <si>
-    <t xml:space="preserve">NETGEAR KIT 1 REG STORES      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NETGEAR NOV POG EMPTY BOXES   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NETGEAR R7800 EMPTY BOX       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW GOOGLE                    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW LOW PRICE TAGS-1000/CS    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW LOYALTY PROGRAM           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW POPSOCKET QRT             </t>
-  </si>
-  <si>
     <t>NIGHT OWL 3CAM DISPLAY BOX KIT</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTEBOOK TRAY                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOV DEC BIC IOM               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NX2500 NON-WORKING DISPLAY    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NXT SURGE                     </t>
-  </si>
-  <si>
     <t>009-047-478-478</t>
   </si>
   <si>
@@ -282,159 +171,48 @@
     <t>PAPER-8X11-110#GLCVR-SHT1200CS</t>
   </si>
   <si>
-    <t xml:space="preserve">PAPER-11X17 NAV 24#-500/RM    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAPER-8.5X14-24#-REAM         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAPER-11X17-24#-REAM          </t>
-  </si>
-  <si>
     <t xml:space="preserve">PAPER-110# 8X11 WHT INDEX-250 </t>
   </si>
   <si>
-    <t xml:space="preserve">PASSPORT PHOTO MEDIA KIT-2PK  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASSPORT PHOTO HEADER SIGN    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASSPORT PHOTO SLEEVE-50PK    </t>
-  </si>
-  <si>
     <t>009-047-446-446</t>
   </si>
   <si>
-    <t xml:space="preserve">REFILL STAPLE TYPE V          </t>
-  </si>
-  <si>
     <t xml:space="preserve">REGISTER ROLLS-EXP3/1/15-50CS </t>
   </si>
   <si>
     <t xml:space="preserve">REPLACEMENT POD HEAD ASSEMBLY </t>
   </si>
   <si>
-    <t xml:space="preserve">RETAIL SOLUTIONS EC LUG ON    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIBBON(3.15IN) - DC USE ONLY  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIBBON-EPSON ERC 31-6/PK      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIBBON-EPSON ERC-32--6/BX     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROBO WRAP - DC USE ONLY       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLL-REGISTER (NEW)-50/CS     </t>
-  </si>
-  <si>
     <t>ROLLS-THERMAL FOR VERIFONE 3PK</t>
   </si>
   <si>
-    <t xml:space="preserve">ROLL TOWEL-GP-6/CS            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ROLL TOWELS-6/CS              </t>
-  </si>
-  <si>
     <t>009-047-443-443</t>
   </si>
   <si>
     <t>009-047-434-434</t>
   </si>
   <si>
-    <t xml:space="preserve">STAMP-2PK-SC Q14 RED-SD       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STAMP-2PK-SC-Q27 BLACK-SD     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STAMP-2PK-SC-Q11 RED-SD       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STAMP-2PK-SC-Q18 RED SD       </t>
-  </si>
-  <si>
     <t xml:space="preserve">STAMP-2PK SC-Q24 RED SAME DAY </t>
   </si>
   <si>
-    <t xml:space="preserve">STAMP-2PK-SC-Q18 BLUE SD      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STANCHION SIGN 22X28          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STANCHION SIGN 16X28          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STAPLE CART 4595/D95/B9100    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STAPLE HOUSE CART. C60/C9070  </t>
-  </si>
-  <si>
     <t>STAPLE REFILLS-C60/70/4595/D95</t>
   </si>
   <si>
-    <t xml:space="preserve">STAPLES BTS BULK GRAPHIC KIT  </t>
-  </si>
-  <si>
     <t>009-047-449-449</t>
   </si>
   <si>
-    <t xml:space="preserve">TABS-MYLAR-1/3 CUT-252/BOX    </t>
-  </si>
-  <si>
     <t xml:space="preserve">TAGHOLDER-2X3 CLEAR FOR T-100 </t>
   </si>
   <si>
     <t xml:space="preserve">TAG HOLDER-2X3 W MAGNET-100PK </t>
   </si>
   <si>
-    <t xml:space="preserve">TAG-OUT OF STOCK (100PK)      </t>
-  </si>
-  <si>
     <t>TAPE DISPENSER-SHIP FROM STORE</t>
   </si>
   <si>
-    <t xml:space="preserve">TAPE-SHIP FROM STORE-8 ROLLS  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAX2 23                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAX CLEARANCE HEADERS         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAX 20 DOVER SIGN KIT 4       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAX 20 DOVER SIGN KIT 5       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAX 20 DOVER SIGN KIT 6       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAX 20 DOVER SIGN KIT 7       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VACUUM BAGS-ROYAL-10PK     </t>
-  </si>
-  <si>
     <t>VACUUM BAGS-SENSOR S12-10PK</t>
   </si>
   <si>
-    <t xml:space="preserve">VIBE MOD PADFOLIO          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VINYL-BLACK                </t>
-  </si>
-  <si>
     <t xml:space="preserve">WF LAM-3MIL GLOSS-25X250-2RLS </t>
   </si>
   <si>
@@ -453,108 +231,30 @@
     <t>WIDE FORMAT BOX-ROLL PRINT-5CS</t>
   </si>
   <si>
-    <t xml:space="preserve">WIDE FORMATBOX-MOUNTED-5/CS   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIN 8 PRO-NOT FOR RESALE DVD  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIPES-ALCOHOL 100 COUNT       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIRE-BAIL WIRE 125PK          </t>
-  </si>
-  <si>
     <t xml:space="preserve">WONDERBOOM DUMMY PK LOGO REFR </t>
   </si>
   <si>
-    <t xml:space="preserve">WRITING PWR BIN-SPR           </t>
-  </si>
-  <si>
     <t>009-047-442-442</t>
   </si>
   <si>
     <t>YELLOW CLEARANCE-5X3/14X3-50PK</t>
   </si>
   <si>
-    <t xml:space="preserve">YELLOW CLEARANCE-BLANK-50/PK  </t>
-  </si>
-  <si>
     <t>ZIP TIES FOR RTW TOTES-100/BAG</t>
   </si>
   <si>
-    <t xml:space="preserve">BAG-2.25MIL-40X28-100/CS      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-2.25MIL-8X40-500/CS       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-M LARGE                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-M SMALL                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-NON WOVEN-50/CS           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-PAPER REGISTER-300/BALE   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-PLASTIC REGISTER-500/CS   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-PLASTIC MED REG-2000CS    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-RACKS(HOLDER) 2PK         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-RECYCLE-SMALL-75/CS       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAG-RECYCLE-LARGE-75/CS       </t>
-  </si>
-  <si>
     <t>BAG-REFILL FOR HP RETRIEVAL UN</t>
   </si>
   <si>
-    <t xml:space="preserve">CREW BOTTLE &amp; TRIGGER         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CREW NACLEANER-1 BTL         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CREW NACLEANER-32OZ EA       </t>
-  </si>
-  <si>
     <t xml:space="preserve">CROSSBAR ARM/CLIP PROMO-10/BX </t>
   </si>
   <si>
-    <t xml:space="preserve">CROSSBAR-4FTX2IN-2PK          </t>
-  </si>
-  <si>
     <t xml:space="preserve">CROSSBAR-1/2INX4FT-FLAT-4/BOX </t>
   </si>
   <si>
     <t>CROSSBAR KIT FORCOLLABORATION</t>
   </si>
   <si>
-    <t xml:space="preserve">CROSSBAR-36X1/2-2/BOX         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CROSSBAR-36X2-2/BOX           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CROSSBAR-36X5-2/BOX           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CROSSBAR-36X11-2/BOX          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CROSSBAR-48X1/2-2/BOX         </t>
-  </si>
-  <si>
     <t>UNISEX RED TEE-2XL-S/S</t>
   </si>
   <si>
@@ -564,141 +264,42 @@
     <t>UNISEX RED TEE-4XL-S/S</t>
   </si>
   <si>
-    <t xml:space="preserve">UNISEX TEE-LG SS      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNISEX TEE-MED SS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNISEX TEE-SM SS      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNISEX TEE-4XL SS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNISEX TEE-2XL SS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNISEX TEE-3XL SS     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNISEX TEE-XL SS      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNISEX TEE-5XL SS     </t>
-  </si>
-  <si>
     <t xml:space="preserve">UNIV DIVIDER ARMS-3PK </t>
   </si>
   <si>
-    <t xml:space="preserve">DISP ASTM LEV 3 MASK-50PK     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISP BUS HOURS OYSTER         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISP-BUSINESS HOURS-SS        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISPENSER-AIR FRESHENER       </t>
-  </si>
-  <si>
     <t>DISPENSER-BUBBLE WRAP 12IN PRF</t>
   </si>
   <si>
-    <t xml:space="preserve">DISPENSER-GP TOILET TISSUE    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISPENSER-KC ROLL TOWEL       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISPENSER-KC TOILET TISSUE    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISPENSER - SOAP              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISPENSER-TOILET SEAT         </t>
-  </si>
-  <si>
     <t>DISPENSER-W/PEANUTS LOOSE FILL</t>
   </si>
   <si>
-    <t xml:space="preserve">DISP FIX POSTER SGN STAND     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EASY REBATE DEMO              </t>
-  </si>
-  <si>
     <t>EASY TECH 2.0 PRODUCTION BOARD</t>
   </si>
   <si>
     <t>EASY TECH SIG MOMENT FOLDER-25</t>
   </si>
   <si>
-    <t xml:space="preserve">EASY TECH TABLET APP-10PK     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EASY TECH TEAR PAD-5/PK       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">E2G PRICE CHANNEL DISPLAY     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMPTY BOX                     </t>
-  </si>
-  <si>
     <t xml:space="preserve">EMPTY BOX-ARLO1080 HD SEC CAM </t>
   </si>
   <si>
     <t xml:space="preserve">EMPTYBOX-ARLO VMC3040S SECCAM </t>
   </si>
   <si>
-    <t xml:space="preserve">EMPTY BOX-ARLO SILICONE SKIN  </t>
-  </si>
-  <si>
     <t xml:space="preserve">EMPTY BOX-ARLO SMART HOME CAM </t>
   </si>
   <si>
     <t>EMPTY BOX-ARLO HD 1 CAMERA KIT</t>
   </si>
   <si>
-    <t xml:space="preserve">FIXTURE-OXO ENDCAP KIT        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIXTURE-OXO GLORIFIER         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIRST-AID TRIANGULAR BANDAGE  </t>
-  </si>
-  <si>
     <t xml:space="preserve">FIX-ADHESIVE VENDOR TAG-25/CS </t>
   </si>
   <si>
-    <t xml:space="preserve">FIXT-5 PACK BINDER VIGNETTE   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIXTUER-OXO SPINNER           </t>
-  </si>
-  <si>
     <t>FIXTURE-BASE DECK SIGN CHANNEL</t>
   </si>
   <si>
-    <t xml:space="preserve">FIXTURE-BBSLIDE DIVIDER GRAY  </t>
-  </si>
-  <si>
     <t>FIXTURE-BBSLIDE DIVIDER OYSTER</t>
   </si>
   <si>
-    <t xml:space="preserve">FIXTURE - DIGITAL VOICE       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIXTURE-GIFT CARD TOWER       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIXTURE - OXO ISLAND DISPLAY  </t>
-  </si>
-  <si>
     <t>GRAY TEE SHIRT-4XL-DMA STORES</t>
   </si>
   <si>
@@ -706,6 +307,405 @@
   </si>
   <si>
     <t>GRAY TEE SHIRT-3XL-DMA STORES</t>
+  </si>
+  <si>
+    <t>AIO DISPLAY MAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIRPODS AUDIO SQUARE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIRTAG PRICE/PULL CARD KIT </t>
+  </si>
+  <si>
+    <t>BAG-2.25MIL-40X28-100/CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-2.25MIL-8X40-500/CS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-M LARGE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-M SMALL </t>
+  </si>
+  <si>
+    <t>BAG-PAPER REGISTER-300/BALE</t>
+  </si>
+  <si>
+    <t>BAG-PLASTIC REGISTER-500/CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-PLASTIC MED REG-2000CS </t>
+  </si>
+  <si>
+    <t>BAG-RACKS(HOLDER) 2PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-RECYCLE-SMALL-75/CS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAG-RECYCLE-LARGE-75/CS </t>
+  </si>
+  <si>
+    <t>CREW BOTTLE &amp; TRIGGER</t>
+  </si>
+  <si>
+    <t>CREW NACLEANER-1 BTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREW NACLEANER-32OZ EA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR-4FTX2IN-2PK </t>
+  </si>
+  <si>
+    <t>CROSSBAR-36X1/2-2/BOX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CROSSBAR-36X11-2/BOX </t>
+  </si>
+  <si>
+    <t>CROSSBAR-48X1/2-2/BOX</t>
+  </si>
+  <si>
+    <t>DISP BUS HOURS OYSTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER-AIR FRESHENER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER-GP TOILET TISSUE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER-KC ROLL TOWEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPENSER-KC TOILET TISSUE </t>
+  </si>
+  <si>
+    <t>DISPENSER-TOILET SEAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EASY TECH TEAR PAD-5/PK </t>
+  </si>
+  <si>
+    <t>EMPTY BOX</t>
+  </si>
+  <si>
+    <t>FIXT-5 PACK BINDER VIGNETTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXTURE - DIGITAL VOICE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIXTURE-GIFT CARD TOWER </t>
+  </si>
+  <si>
+    <t>FIXTURE-OXO GLORIFIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAND SANITIZER-24/CS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAND WRAP - DC USE ONLY </t>
+  </si>
+  <si>
+    <t>HO22ET5150 SIGN</t>
+  </si>
+  <si>
+    <t>NEW GOOGLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW LOYALTY PROGRAM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NXT SURGE </t>
+  </si>
+  <si>
+    <t>PAPER-11X17-24#-REAM</t>
+  </si>
+  <si>
+    <t>REFILL STAPLE TYPE V</t>
+  </si>
+  <si>
+    <t>STANCHION SIGN 22X28</t>
+  </si>
+  <si>
+    <t>STANCHION SIGN 16X28</t>
+  </si>
+  <si>
+    <t>VIBE MOD PADFOLIO</t>
+  </si>
+  <si>
+    <t>WIRE-BAIL WIRE 125PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WRITING PWR BIN-SPR </t>
+  </si>
+  <si>
+    <t>ACADEMY ACRYLIC RACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NETGEAR KIT 1 REG STORES </t>
+  </si>
+  <si>
+    <t>NOV DEC BIC IOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIBBON-EPSON ERC 31-6/PK </t>
+  </si>
+  <si>
+    <t>RIBBON-EPSON ERC-32--6/BX</t>
+  </si>
+  <si>
+    <t>ROLL-REGISTER (NEW)-50/CS</t>
+  </si>
+  <si>
+    <t>STAMP-2PK-SC-Q27 BLACK-SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STAMP-2PK-SC-Q18 BLUE SD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAG-OUT OF STOCK (100PK) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-LG SS </t>
+  </si>
+  <si>
+    <t>UNISEX TEE-MED SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-SM SS </t>
+  </si>
+  <si>
+    <t>UNISEX TEE-4XL SS</t>
+  </si>
+  <si>
+    <t>UNISEX TEE-2XL SS</t>
+  </si>
+  <si>
+    <t>UNISEX TEE-3XL SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNISEX TEE-XL SS </t>
+  </si>
+  <si>
+    <t>UNISEX TEE-5XL SS</t>
+  </si>
+  <si>
+    <t>VACUUM BAGS-ROYAL-10PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VINYL-BLACK </t>
+  </si>
+  <si>
+    <t>ACRYLIC-SMALL CALCULATOR TBD</t>
+  </si>
+  <si>
+    <t>A2 DOUBLE FRONT END (2PANEL)</t>
+  </si>
+  <si>
+    <t>BAG-NON WOVEN-50/CS</t>
+  </si>
+  <si>
+    <t>CROSSBAR-36X2-2/BOX</t>
+  </si>
+  <si>
+    <t>CROSSBAR-36X5-2/BOX</t>
+  </si>
+  <si>
+    <t>DISP ASTM LEV 3 MASK-50PK</t>
+  </si>
+  <si>
+    <t>DISP-BUSINESS HOURS-SS</t>
+  </si>
+  <si>
+    <t>DISPENSER - SOAP</t>
+  </si>
+  <si>
+    <t>DISP FIX POSTER SGN STAND</t>
+  </si>
+  <si>
+    <t>EASY REBATE DEMO</t>
+  </si>
+  <si>
+    <t>EASY TECH TABLET APP-10PK</t>
+  </si>
+  <si>
+    <t>E2G PRICE CHANNEL DISPLAY</t>
+  </si>
+  <si>
+    <t>EMPTY BOX-ARLO SILICONE SKIN</t>
+  </si>
+  <si>
+    <t>FIRST-AID TRIANGULAR BANDAGE</t>
+  </si>
+  <si>
+    <t>FIXTUER-OXO SPINNER</t>
+  </si>
+  <si>
+    <t>FIXTURE-BBSLIDE DIVIDER GRAY</t>
+  </si>
+  <si>
+    <t>FIXTURE - OXO ISLAND DISPLAY</t>
+  </si>
+  <si>
+    <t>FIXTURE-OXO ENDCAP KIT</t>
+  </si>
+  <si>
+    <t>HAND SANITIZER-1 GAL-75% ALC</t>
+  </si>
+  <si>
+    <t>HAND TRUCK</t>
+  </si>
+  <si>
+    <t>H22 DECO CALENDAR TRAY</t>
+  </si>
+  <si>
+    <t>HIGH-DEFINITION MEDIA PLAYER</t>
+  </si>
+  <si>
+    <t>HIGH WALL USB SIGNAGE KIT</t>
+  </si>
+  <si>
+    <t>HINGE-ELMERS-2PK</t>
+  </si>
+  <si>
+    <t>HOL19 ACER</t>
+  </si>
+  <si>
+    <t>LABEL-MA PRICE CHECKER-12RLS</t>
+  </si>
+  <si>
+    <t>LABEL-MATTE 4UP-5X3 OVAL-100</t>
+  </si>
+  <si>
+    <t>LABEL-PC WRAP-EZ TECH-500/RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LABEL-RECYCLE-500/ROLL </t>
+  </si>
+  <si>
+    <t>LABEL-TECH RETURN 5X4-800/RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LABEL-22UP-100/PK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LABEL UPS A-CAE1-500RL </t>
+  </si>
+  <si>
+    <t>MANAGER WMNS POLO-S-LS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NETGEAR NOV POG EMPTY BOXES </t>
+  </si>
+  <si>
+    <t>NETGEAR R7800 EMPTY BOX</t>
+  </si>
+  <si>
+    <t>NEW LOW PRICE TAGS-1000/CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW POPSOCKET QRT </t>
+  </si>
+  <si>
+    <t>NOTEBOOK TRAY</t>
+  </si>
+  <si>
+    <t>NX2500 NON-WORKING DISPLAY</t>
+  </si>
+  <si>
+    <t>PAPER-11X17 NAV 24#-500/RM</t>
+  </si>
+  <si>
+    <t>PAPER-8.5X14-24#-REAM</t>
+  </si>
+  <si>
+    <t>PASSPORT PHOTO MEDIA KIT-2PK</t>
+  </si>
+  <si>
+    <t>PASSPORT PHOTO HEADER SIGN</t>
+  </si>
+  <si>
+    <t>PASSPORT PHOTO SLEEVE-50PK</t>
+  </si>
+  <si>
+    <t>RETAIL SOLUTIONS EC LUG ON</t>
+  </si>
+  <si>
+    <t>RIBBON(3.15IN) - DC USE ONLY</t>
+  </si>
+  <si>
+    <t>ROBO WRAP - DC USE ONLY</t>
+  </si>
+  <si>
+    <t>ROLL TOWEL-GP-6/CS</t>
+  </si>
+  <si>
+    <t>ROLL TOWELS-6/CS</t>
+  </si>
+  <si>
+    <t>STAMP-2PK-SC Q14 RED-SD</t>
+  </si>
+  <si>
+    <t>STAMP-2PK-SC-Q11 RED-SD</t>
+  </si>
+  <si>
+    <t>STAMP-2PK-SC-Q18 RED SD</t>
+  </si>
+  <si>
+    <t>STAPLE CART 4595/D95/B9100</t>
+  </si>
+  <si>
+    <t>STAPLE HOUSE CART. C60/C9070</t>
+  </si>
+  <si>
+    <t>STAPLES BTS BULK GRAPHIC KIT</t>
+  </si>
+  <si>
+    <t>TABS-MYLAR-1/3 CUT-252/BOX</t>
+  </si>
+  <si>
+    <t>TAPE-SHIP FROM STORE-8 ROLLS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAX2 23 </t>
+  </si>
+  <si>
+    <t>TAX CLEARANCE HEADERS</t>
+  </si>
+  <si>
+    <t>TAX 20 DOVER SIGN KIT 4</t>
+  </si>
+  <si>
+    <t>TAX 20 DOVER SIGN KIT 5</t>
+  </si>
+  <si>
+    <t>TAX 20 DOVER SIGN KIT 6</t>
+  </si>
+  <si>
+    <t>TAX 20 DOVER SIGN KIT 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIDE FORMATBOX-MOUNTED-5/CS </t>
+  </si>
+  <si>
+    <t>WIN 8 PRO-NOT FOR RESALE DVD</t>
+  </si>
+  <si>
+    <t>WIPES-ALCOHOL 100 COUNT</t>
+  </si>
+  <si>
+    <t>YELLOW CLEARANCE-BLANK-50/PK</t>
+  </si>
+  <si>
+    <t>ACADEMY OIL RACK</t>
+  </si>
+  <si>
+    <t>744788 AC BOX</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1075,7 @@
   <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1105,13 +1105,13 @@
         <v>2636750</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="C2">
         <v>0.01</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1119,13 +1119,13 @@
         <v>2636751</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>222</v>
       </c>
       <c r="C3">
         <v>0.01</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1133,13 +1133,13 @@
         <v>861198</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>223</v>
       </c>
       <c r="C4">
         <v>0.01</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1147,13 +1147,13 @@
         <v>680462</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="C5">
         <v>4.5</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1161,13 +1161,13 @@
         <v>581080</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>26.16</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1175,13 +1175,13 @@
         <v>721047</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>31.95</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1189,13 +1189,13 @@
         <v>797995</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="C8">
         <v>0.01</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1203,13 +1203,13 @@
         <v>2554453</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="C9">
         <v>0.01</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1217,13 +1217,13 @@
         <v>1944628</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>0.01</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1231,13 +1231,13 @@
         <v>24375279</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>0.01</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1245,13 +1245,13 @@
         <v>24462109</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="C12">
         <v>0.01</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1259,13 +1259,13 @@
         <v>24507841</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="C13">
         <v>0.01</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1273,13 +1273,13 @@
         <v>120565</v>
       </c>
       <c r="B14" t="s">
-        <v>149</v>
+        <v>94</v>
       </c>
       <c r="C14">
         <v>39.5</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1287,13 +1287,13 @@
         <v>120566</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="C15">
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1301,13 +1301,13 @@
         <v>753865</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>96</v>
       </c>
       <c r="C16">
         <v>0.01</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1315,13 +1315,13 @@
         <v>753864</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>97</v>
       </c>
       <c r="C17">
         <v>0.01</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1329,13 +1329,13 @@
         <v>2103529</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C18">
         <v>0.01</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1343,13 +1343,13 @@
         <v>830474</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="C19">
         <v>46.55</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1357,13 +1357,13 @@
         <v>820222</v>
       </c>
       <c r="B20" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="C20">
         <v>49.29</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1371,13 +1371,13 @@
         <v>24486274</v>
       </c>
       <c r="B21" t="s">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="C21">
         <v>43.45</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1385,13 +1385,13 @@
         <v>489906</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>101</v>
       </c>
       <c r="C22">
         <v>59.16</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1399,13 +1399,13 @@
         <v>698387</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>102</v>
       </c>
       <c r="C23">
         <v>14.54</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1413,13 +1413,13 @@
         <v>698389</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="C24">
         <v>35.21</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1427,13 +1427,13 @@
         <v>387288</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>69</v>
       </c>
       <c r="C25">
         <v>0.01</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1441,13 +1441,13 @@
         <v>375782</v>
       </c>
       <c r="B26" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="C26">
         <v>0.37</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1455,13 +1455,13 @@
         <v>477808</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
       <c r="C27">
         <v>23.75</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1469,13 +1469,13 @@
         <v>24441152</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>106</v>
       </c>
       <c r="C28">
         <v>1.56</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1483,13 +1483,13 @@
         <v>122718</v>
       </c>
       <c r="B29" t="s">
-        <v>164</v>
+        <v>70</v>
       </c>
       <c r="C29">
         <v>29.55</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1497,13 +1497,13 @@
         <v>24399258</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="C30">
         <v>0.01</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1511,13 +1511,13 @@
         <v>1921941</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>71</v>
       </c>
       <c r="C31">
         <v>0.01</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1525,13 +1525,13 @@
         <v>24522078</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>72</v>
       </c>
       <c r="C32">
         <v>0.01</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1539,13 +1539,13 @@
         <v>1924772</v>
       </c>
       <c r="B33" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="C33">
         <v>0.01</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1553,13 +1553,13 @@
         <v>1924773</v>
       </c>
       <c r="B34" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C34">
         <v>0.01</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1567,13 +1567,13 @@
         <v>1924774</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C35">
         <v>0.01</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1581,13 +1581,13 @@
         <v>1924775</v>
       </c>
       <c r="B36" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="C36">
         <v>0.01</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1595,13 +1595,13 @@
         <v>1924776</v>
       </c>
       <c r="B37" t="s">
-        <v>172</v>
+        <v>110</v>
       </c>
       <c r="C37">
         <v>0.01</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1609,13 +1609,13 @@
         <v>24520258</v>
       </c>
       <c r="B38" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="C38">
         <v>5.5</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1623,13 +1623,13 @@
         <v>399890</v>
       </c>
       <c r="B39" t="s">
-        <v>186</v>
+        <v>111</v>
       </c>
       <c r="C39">
         <v>0.01</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1637,13 +1637,13 @@
         <v>399198</v>
       </c>
       <c r="B40" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="C40">
         <v>0.01</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1651,13 +1651,13 @@
         <v>674158</v>
       </c>
       <c r="B41" t="s">
-        <v>188</v>
+        <v>112</v>
       </c>
       <c r="C41">
         <v>28</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1665,13 +1665,13 @@
         <v>396538</v>
       </c>
       <c r="B42" t="s">
-        <v>189</v>
+        <v>77</v>
       </c>
       <c r="C42">
         <v>17.75</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1679,13 +1679,13 @@
         <v>385169</v>
       </c>
       <c r="B43" t="s">
-        <v>190</v>
+        <v>113</v>
       </c>
       <c r="C43">
         <v>0.01</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1693,13 +1693,13 @@
         <v>918748</v>
       </c>
       <c r="B44" t="s">
-        <v>191</v>
+        <v>114</v>
       </c>
       <c r="C44">
         <v>0.01</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1707,13 +1707,13 @@
         <v>2758595</v>
       </c>
       <c r="B45" t="s">
-        <v>192</v>
+        <v>115</v>
       </c>
       <c r="C45">
         <v>0.01</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1721,13 +1721,13 @@
         <v>919623</v>
       </c>
       <c r="B46" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
       <c r="C46">
         <v>0.01</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1735,13 +1735,13 @@
         <v>385163</v>
       </c>
       <c r="B47" t="s">
-        <v>194</v>
+        <v>116</v>
       </c>
       <c r="C47">
         <v>5.13</v>
       </c>
       <c r="D47" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1749,13 +1749,13 @@
         <v>396540</v>
       </c>
       <c r="B48" t="s">
-        <v>195</v>
+        <v>78</v>
       </c>
       <c r="C48">
         <v>11.69</v>
       </c>
       <c r="D48" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1763,13 +1763,13 @@
         <v>2843067</v>
       </c>
       <c r="B49" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
       <c r="C49">
         <v>0.01</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1777,13 +1777,13 @@
         <v>746309</v>
       </c>
       <c r="B50" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="C50">
         <v>0.01</v>
       </c>
       <c r="D50" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1791,13 +1791,13 @@
         <v>902635</v>
       </c>
       <c r="B51" t="s">
-        <v>198</v>
+        <v>79</v>
       </c>
       <c r="C51">
         <v>198.48</v>
       </c>
       <c r="D51" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1805,13 +1805,13 @@
         <v>798378</v>
       </c>
       <c r="B52" t="s">
-        <v>199</v>
+        <v>80</v>
       </c>
       <c r="C52">
         <v>22.05</v>
       </c>
       <c r="D52" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1819,13 +1819,13 @@
         <v>163433</v>
       </c>
       <c r="B53" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="C53">
         <v>0.01</v>
       </c>
       <c r="D53" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1833,13 +1833,13 @@
         <v>358954</v>
       </c>
       <c r="B54" t="s">
-        <v>201</v>
+        <v>117</v>
       </c>
       <c r="C54">
         <v>6.33</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1847,13 +1847,13 @@
         <v>130442</v>
       </c>
       <c r="B55" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="C55">
         <v>0.01</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1861,13 +1861,13 @@
         <v>1571565</v>
       </c>
       <c r="B56" t="s">
-        <v>203</v>
+        <v>118</v>
       </c>
       <c r="C56">
         <v>0.01</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1875,13 +1875,13 @@
         <v>24401194</v>
       </c>
       <c r="B57" t="s">
-        <v>204</v>
+        <v>81</v>
       </c>
       <c r="C57">
         <v>0.01</v>
       </c>
       <c r="D57" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1889,13 +1889,13 @@
         <v>24401195</v>
       </c>
       <c r="B58" t="s">
-        <v>205</v>
+        <v>82</v>
       </c>
       <c r="C58">
         <v>0.01</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1903,13 +1903,13 @@
         <v>24401196</v>
       </c>
       <c r="B59" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="C59">
         <v>0.01</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1917,13 +1917,13 @@
         <v>24401197</v>
       </c>
       <c r="B60" t="s">
-        <v>207</v>
+        <v>83</v>
       </c>
       <c r="C60">
         <v>0.01</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1931,13 +1931,13 @@
         <v>24401198</v>
       </c>
       <c r="B61" t="s">
-        <v>208</v>
+        <v>84</v>
       </c>
       <c r="C61">
         <v>0.01</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1945,13 +1945,13 @@
         <v>485797</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="C62">
         <v>0.49</v>
       </c>
       <c r="D62" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1959,13 +1959,13 @@
         <v>668364</v>
       </c>
       <c r="B63" t="s">
-        <v>212</v>
+        <v>85</v>
       </c>
       <c r="C63">
         <v>62.5</v>
       </c>
       <c r="D63" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1973,13 +1973,13 @@
         <v>737795</v>
       </c>
       <c r="B64" t="s">
-        <v>213</v>
+        <v>119</v>
       </c>
       <c r="C64">
         <v>0.01</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1987,13 +1987,13 @@
         <v>791654</v>
       </c>
       <c r="B65" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
       <c r="C65">
         <v>0.01</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2001,13 +2001,13 @@
         <v>821806</v>
       </c>
       <c r="B66" t="s">
-        <v>215</v>
+        <v>86</v>
       </c>
       <c r="C66">
         <v>0.01</v>
       </c>
       <c r="D66" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2015,13 +2015,13 @@
         <v>797525</v>
       </c>
       <c r="B67" t="s">
-        <v>216</v>
+        <v>170</v>
       </c>
       <c r="C67">
         <v>0.01</v>
       </c>
       <c r="D67" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2029,13 +2029,13 @@
         <v>797527</v>
       </c>
       <c r="B68" t="s">
-        <v>217</v>
+        <v>87</v>
       </c>
       <c r="C68">
         <v>0.01</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2043,13 +2043,13 @@
         <v>791718</v>
       </c>
       <c r="B69" t="s">
-        <v>218</v>
+        <v>120</v>
       </c>
       <c r="C69">
         <v>0.01</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2057,13 +2057,13 @@
         <v>764677</v>
       </c>
       <c r="B70" t="s">
-        <v>219</v>
+        <v>121</v>
       </c>
       <c r="C70">
         <v>0.01</v>
       </c>
       <c r="D70" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2071,13 +2071,13 @@
         <v>781812</v>
       </c>
       <c r="B71" t="s">
-        <v>220</v>
+        <v>171</v>
       </c>
       <c r="C71">
         <v>0.01</v>
       </c>
       <c r="D71" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2085,13 +2085,13 @@
         <v>791655</v>
       </c>
       <c r="B72" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="C72">
         <v>0.01</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2099,13 +2099,13 @@
         <v>814168</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>122</v>
       </c>
       <c r="C73">
         <v>0.01</v>
       </c>
       <c r="D73" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2113,13 +2113,13 @@
         <v>24430271</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>88</v>
       </c>
       <c r="C74">
         <v>0.01</v>
       </c>
       <c r="D74" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2127,13 +2127,13 @@
         <v>24430272</v>
       </c>
       <c r="B75" t="s">
-        <v>222</v>
+        <v>89</v>
       </c>
       <c r="C75">
         <v>0.01</v>
       </c>
       <c r="D75" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2141,13 +2141,13 @@
         <v>24430273</v>
       </c>
       <c r="B76" t="s">
-        <v>223</v>
+        <v>90</v>
       </c>
       <c r="C76">
         <v>0.01</v>
       </c>
       <c r="D76" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2155,13 +2155,13 @@
         <v>24430274</v>
       </c>
       <c r="B77" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C77">
         <v>0.01</v>
       </c>
       <c r="D77" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2169,13 +2169,13 @@
         <v>24430275</v>
       </c>
       <c r="B78" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C78">
         <v>0.01</v>
       </c>
       <c r="D78" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2183,13 +2183,13 @@
         <v>24479433</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C79">
         <v>0.01</v>
       </c>
       <c r="D79" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2197,13 +2197,13 @@
         <v>24443470</v>
       </c>
       <c r="B80" t="s">
-        <v>25</v>
+        <v>123</v>
       </c>
       <c r="C80">
         <v>97.37</v>
       </c>
       <c r="D80" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2211,13 +2211,13 @@
         <v>24449149</v>
       </c>
       <c r="B81" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="C81">
         <v>23</v>
       </c>
       <c r="D81" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2225,13 +2225,13 @@
         <v>1056170</v>
       </c>
       <c r="B82" t="s">
-        <v>27</v>
+        <v>174</v>
       </c>
       <c r="C82">
         <v>0.01</v>
       </c>
       <c r="D82" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2239,13 +2239,13 @@
         <v>749931</v>
       </c>
       <c r="B83" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="C83">
         <v>0.01</v>
       </c>
       <c r="D83" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2253,13 +2253,13 @@
         <v>24547928</v>
       </c>
       <c r="B84" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="C84">
         <v>0.01</v>
       </c>
       <c r="D84" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2267,13 +2267,13 @@
         <v>2115890</v>
       </c>
       <c r="B85" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C85">
         <v>0.01</v>
       </c>
       <c r="D85" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2281,13 +2281,13 @@
         <v>24500475</v>
       </c>
       <c r="B86" t="s">
-        <v>31</v>
+        <v>176</v>
       </c>
       <c r="C86">
         <v>0.01</v>
       </c>
       <c r="D86" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2295,13 +2295,13 @@
         <v>930831</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C87">
         <v>0.01</v>
       </c>
       <c r="D87" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2309,13 +2309,13 @@
         <v>2112627</v>
       </c>
       <c r="B88" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="C88">
         <v>0.01</v>
       </c>
       <c r="D88" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2323,13 +2323,13 @@
         <v>761485</v>
       </c>
       <c r="B89" t="s">
-        <v>34</v>
+        <v>178</v>
       </c>
       <c r="C89">
         <v>1.4</v>
       </c>
       <c r="D89" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2337,13 +2337,13 @@
         <v>24539938</v>
       </c>
       <c r="B90" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="C90">
         <v>0.01</v>
       </c>
       <c r="D90" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2351,13 +2351,13 @@
         <v>24421441</v>
       </c>
       <c r="B91" t="s">
-        <v>36</v>
+        <v>179</v>
       </c>
       <c r="C91">
         <v>0.01</v>
       </c>
       <c r="D91" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2365,13 +2365,13 @@
         <v>571594</v>
       </c>
       <c r="B92" t="s">
-        <v>39</v>
+        <v>180</v>
       </c>
       <c r="C92">
         <v>99</v>
       </c>
       <c r="D92" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2379,13 +2379,13 @@
         <v>24473027</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C93">
         <v>13.34</v>
       </c>
       <c r="D93" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2393,13 +2393,13 @@
         <v>24473028</v>
       </c>
       <c r="B94" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="C94">
         <v>12.32</v>
       </c>
       <c r="D94" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2407,13 +2407,13 @@
         <v>24473029</v>
       </c>
       <c r="B95" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C95">
         <v>13.35</v>
       </c>
       <c r="D95" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2421,13 +2421,13 @@
         <v>24473030</v>
       </c>
       <c r="B96" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C96">
         <v>13.23</v>
       </c>
       <c r="D96" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2435,13 +2435,13 @@
         <v>674505</v>
       </c>
       <c r="B97" t="s">
-        <v>44</v>
+        <v>182</v>
       </c>
       <c r="C97">
         <v>5.75</v>
       </c>
       <c r="D97" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2449,13 +2449,13 @@
         <v>697353</v>
       </c>
       <c r="B98" t="s">
-        <v>45</v>
+        <v>183</v>
       </c>
       <c r="C98">
         <v>6.57</v>
       </c>
       <c r="D98" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -2463,13 +2463,13 @@
         <v>439837</v>
       </c>
       <c r="B99" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C99">
         <v>4.8600000000000003</v>
       </c>
       <c r="D99" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -2477,13 +2477,13 @@
         <v>382583</v>
       </c>
       <c r="B100" t="s">
-        <v>47</v>
+        <v>184</v>
       </c>
       <c r="C100">
         <v>18.66</v>
       </c>
       <c r="D100" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -2491,13 +2491,13 @@
         <v>492754</v>
       </c>
       <c r="B101" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C101">
         <v>4.8499999999999996</v>
       </c>
       <c r="D101" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2505,13 +2505,13 @@
         <v>747916</v>
       </c>
       <c r="B102" t="s">
-        <v>49</v>
+        <v>185</v>
       </c>
       <c r="C102">
         <v>10.85</v>
       </c>
       <c r="D102" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -2519,13 +2519,13 @@
         <v>24581460</v>
       </c>
       <c r="B103" t="s">
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="C103">
         <v>0.01</v>
       </c>
       <c r="D103" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2533,13 +2533,13 @@
         <v>868617</v>
       </c>
       <c r="B104" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C104">
         <v>13.76</v>
       </c>
       <c r="D104" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2547,13 +2547,13 @@
         <v>868618</v>
       </c>
       <c r="B105" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C105">
         <v>13.76</v>
       </c>
       <c r="D105" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2561,13 +2561,13 @@
         <v>868619</v>
       </c>
       <c r="B106" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C106">
         <v>13.77</v>
       </c>
       <c r="D106" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2575,13 +2575,13 @@
         <v>868621</v>
       </c>
       <c r="B107" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C107">
         <v>13.76</v>
       </c>
       <c r="D107" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2589,13 +2589,13 @@
         <v>868622</v>
       </c>
       <c r="B108" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="C108">
         <v>14.73</v>
       </c>
       <c r="D108" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2603,13 +2603,13 @@
         <v>868623</v>
       </c>
       <c r="B109" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C109">
         <v>13.76</v>
       </c>
       <c r="D109" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2617,13 +2617,13 @@
         <v>868656</v>
       </c>
       <c r="B110" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C110">
         <v>10.1</v>
       </c>
       <c r="D110" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2631,13 +2631,13 @@
         <v>24374440</v>
       </c>
       <c r="B111" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C111">
         <v>13.76</v>
       </c>
       <c r="D111" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2645,13 +2645,13 @@
         <v>24374441</v>
       </c>
       <c r="B112" t="s">
-        <v>60</v>
+        <v>187</v>
       </c>
       <c r="C112">
         <v>13.96</v>
       </c>
       <c r="D112" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2659,13 +2659,13 @@
         <v>24374442</v>
       </c>
       <c r="B113" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C113">
         <v>13.76</v>
       </c>
       <c r="D113" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2673,13 +2673,13 @@
         <v>24374443</v>
       </c>
       <c r="B114" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C114">
         <v>13.76</v>
       </c>
       <c r="D114" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2687,13 +2687,13 @@
         <v>24374444</v>
       </c>
       <c r="B115" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C115">
         <v>13.76</v>
       </c>
       <c r="D115" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2701,13 +2701,13 @@
         <v>404427</v>
       </c>
       <c r="B116" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="C116">
         <v>0.01</v>
       </c>
       <c r="D116" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -2715,13 +2715,13 @@
         <v>307201</v>
       </c>
       <c r="B117" t="s">
-        <v>65</v>
+        <v>188</v>
       </c>
       <c r="C117">
         <v>0.01</v>
       </c>
       <c r="D117" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -2729,13 +2729,13 @@
         <v>2126719</v>
       </c>
       <c r="B118" t="s">
-        <v>66</v>
+        <v>189</v>
       </c>
       <c r="C118">
         <v>0.01</v>
       </c>
       <c r="D118" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -2743,13 +2743,13 @@
         <v>24375375</v>
       </c>
       <c r="B119" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="C119">
         <v>0.01</v>
       </c>
       <c r="D119" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -2757,13 +2757,13 @@
         <v>271715</v>
       </c>
       <c r="B120" t="s">
-        <v>68</v>
+        <v>190</v>
       </c>
       <c r="C120">
         <v>0.01</v>
       </c>
       <c r="D120" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -2771,13 +2771,13 @@
         <v>24567572</v>
       </c>
       <c r="B121" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="C121">
         <v>0.01</v>
       </c>
       <c r="D121" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -2785,13 +2785,13 @@
         <v>24387510</v>
       </c>
       <c r="B122" t="s">
-        <v>70</v>
+        <v>191</v>
       </c>
       <c r="C122">
         <v>0.01</v>
       </c>
       <c r="D122" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -2799,13 +2799,13 @@
         <v>1230742</v>
       </c>
       <c r="B123" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="C123">
         <v>0.01</v>
       </c>
       <c r="D123" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -2813,13 +2813,13 @@
         <v>24319699</v>
       </c>
       <c r="B124" t="s">
-        <v>72</v>
+        <v>192</v>
       </c>
       <c r="C124">
         <v>0.01</v>
       </c>
       <c r="D124" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -2827,13 +2827,13 @@
         <v>24373366</v>
       </c>
       <c r="B125" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="C125">
         <v>0.01</v>
       </c>
       <c r="D125" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -2841,13 +2841,13 @@
         <v>24526646</v>
       </c>
       <c r="B126" t="s">
-        <v>74</v>
+        <v>193</v>
       </c>
       <c r="C126">
         <v>0.01</v>
       </c>
       <c r="D126" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -2855,13 +2855,13 @@
         <v>24401869</v>
       </c>
       <c r="B127" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="C127">
         <v>0.01</v>
       </c>
       <c r="D127" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -2869,13 +2869,13 @@
         <v>24399270</v>
       </c>
       <c r="B128" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C128">
         <v>79.48</v>
       </c>
       <c r="D128" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -2883,13 +2883,13 @@
         <v>24399271</v>
       </c>
       <c r="B129" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="C129">
         <v>118.63</v>
       </c>
       <c r="D129" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -2897,13 +2897,13 @@
         <v>24399272</v>
       </c>
       <c r="B130" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="C130">
         <v>118.76</v>
       </c>
       <c r="D130" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -2911,13 +2911,13 @@
         <v>24399275</v>
       </c>
       <c r="B131" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C131">
         <v>79.400000000000006</v>
       </c>
       <c r="D131" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -2925,13 +2925,13 @@
         <v>24503275</v>
       </c>
       <c r="B132" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="C132">
         <v>102.04</v>
       </c>
       <c r="D132" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -2939,13 +2939,13 @@
         <v>426227</v>
       </c>
       <c r="B133" t="s">
-        <v>82</v>
+        <v>194</v>
       </c>
       <c r="C133">
         <v>15.8</v>
       </c>
       <c r="D133" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -2953,13 +2953,13 @@
         <v>810026</v>
       </c>
       <c r="B134" t="s">
-        <v>83</v>
+        <v>195</v>
       </c>
       <c r="C134">
         <v>7.97</v>
       </c>
       <c r="D134" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -2967,13 +2967,13 @@
         <v>810029</v>
       </c>
       <c r="B135" t="s">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="C135">
         <v>10.98</v>
       </c>
       <c r="D135" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -2981,13 +2981,13 @@
         <v>24507652</v>
       </c>
       <c r="B136" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="C136">
         <v>9.89</v>
       </c>
       <c r="D136" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -2995,13 +2995,13 @@
         <v>24522057</v>
       </c>
       <c r="B137" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="C137">
         <v>750</v>
       </c>
       <c r="D137" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -3009,13 +3009,13 @@
         <v>24522747</v>
       </c>
       <c r="B138" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="C138">
         <v>0.01</v>
       </c>
       <c r="D138" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -3023,13 +3023,13 @@
         <v>24525624</v>
       </c>
       <c r="B139" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="C139">
         <v>12.84</v>
       </c>
       <c r="D139" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -3037,13 +3037,13 @@
         <v>24508926</v>
       </c>
       <c r="B140" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="C140">
         <v>0.01</v>
       </c>
       <c r="D140" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -3051,13 +3051,13 @@
         <v>1437976</v>
       </c>
       <c r="B141" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="C141">
         <v>57.95</v>
       </c>
       <c r="D141" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -3065,13 +3065,13 @@
         <v>788568</v>
       </c>
       <c r="B142" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="C142">
         <v>44.96</v>
       </c>
       <c r="D142" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -3079,13 +3079,13 @@
         <v>24296490</v>
       </c>
       <c r="B143" t="s">
-        <v>93</v>
+        <v>199</v>
       </c>
       <c r="C143">
         <v>0.01</v>
       </c>
       <c r="D143" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -3093,13 +3093,13 @@
         <v>750022</v>
       </c>
       <c r="B144" t="s">
-        <v>94</v>
+        <v>200</v>
       </c>
       <c r="C144">
         <v>0.01</v>
       </c>
       <c r="D144" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -3107,13 +3107,13 @@
         <v>459125</v>
       </c>
       <c r="B145" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C145">
         <v>8.52</v>
       </c>
       <c r="D145" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -3121,13 +3121,13 @@
         <v>816222</v>
       </c>
       <c r="B146" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="C146">
         <v>8.52</v>
       </c>
       <c r="D146" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -3135,13 +3135,13 @@
         <v>749905</v>
       </c>
       <c r="B147" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
       <c r="C147">
         <v>0.01</v>
       </c>
       <c r="D147" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -3149,13 +3149,13 @@
         <v>2707926</v>
       </c>
       <c r="B148" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C148">
         <v>87.53</v>
       </c>
       <c r="D148" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -3163,13 +3163,13 @@
         <v>580556</v>
       </c>
       <c r="B149" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="C149">
         <v>1.06</v>
       </c>
       <c r="D149" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -3177,13 +3177,13 @@
         <v>918563</v>
       </c>
       <c r="B150" t="s">
-        <v>100</v>
+        <v>202</v>
       </c>
       <c r="C150">
         <v>25.35</v>
       </c>
       <c r="D150" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -3191,13 +3191,13 @@
         <v>24441153</v>
       </c>
       <c r="B151" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="C151">
         <v>41.08</v>
       </c>
       <c r="D151" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -3205,13 +3205,13 @@
         <v>24520544</v>
       </c>
       <c r="B152" t="s">
-        <v>104</v>
+        <v>204</v>
       </c>
       <c r="C152">
         <v>16.22</v>
       </c>
       <c r="D152" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -3219,13 +3219,13 @@
         <v>24522741</v>
       </c>
       <c r="B153" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="C153">
         <v>29.06</v>
       </c>
       <c r="D153" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -3233,13 +3233,13 @@
         <v>24528564</v>
       </c>
       <c r="B154" t="s">
-        <v>106</v>
+        <v>205</v>
       </c>
       <c r="C154">
         <v>16.43</v>
       </c>
       <c r="D154" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -3247,13 +3247,13 @@
         <v>24531210</v>
       </c>
       <c r="B155" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="C155">
         <v>17.09</v>
       </c>
       <c r="D155" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -3261,13 +3261,13 @@
         <v>24531655</v>
       </c>
       <c r="B156" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
       <c r="C156">
         <v>19.940000000000001</v>
       </c>
       <c r="D156" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -3275,13 +3275,13 @@
         <v>24533744</v>
       </c>
       <c r="B157" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="C157">
         <v>17.100000000000001</v>
       </c>
       <c r="D157" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -3289,13 +3289,13 @@
         <v>427724</v>
       </c>
       <c r="B158" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="C158">
         <v>0.01</v>
       </c>
       <c r="D158" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -3303,13 +3303,13 @@
         <v>1958186</v>
       </c>
       <c r="B159" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="C159">
         <v>0.01</v>
       </c>
       <c r="D159" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -3317,13 +3317,13 @@
         <v>721049</v>
       </c>
       <c r="B160" t="s">
-        <v>112</v>
+        <v>207</v>
       </c>
       <c r="C160">
         <v>180.91</v>
       </c>
       <c r="D160" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -3331,13 +3331,13 @@
         <v>369636</v>
       </c>
       <c r="B161" t="s">
-        <v>113</v>
+        <v>208</v>
       </c>
       <c r="C161">
         <v>126.78</v>
       </c>
       <c r="D161" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -3345,13 +3345,13 @@
         <v>710729</v>
       </c>
       <c r="B162" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="C162">
         <v>191.58</v>
       </c>
       <c r="D162" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -3359,13 +3359,13 @@
         <v>800330</v>
       </c>
       <c r="B163" t="s">
-        <v>115</v>
+        <v>209</v>
       </c>
       <c r="C163">
         <v>0.01</v>
       </c>
       <c r="D163" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -3373,13 +3373,13 @@
         <v>404270</v>
       </c>
       <c r="B164" t="s">
-        <v>117</v>
+        <v>210</v>
       </c>
       <c r="C164">
         <v>16.059999999999999</v>
       </c>
       <c r="D164" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3387,13 +3387,13 @@
         <v>596695</v>
       </c>
       <c r="B165" t="s">
-        <v>118</v>
+        <v>55</v>
       </c>
       <c r="C165">
         <v>10.91</v>
       </c>
       <c r="D165" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -3401,13 +3401,13 @@
         <v>24338269</v>
       </c>
       <c r="B166" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="C166">
         <v>46.94</v>
       </c>
       <c r="D166" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -3415,13 +3415,13 @@
         <v>561287</v>
       </c>
       <c r="B167" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="C167">
         <v>5.1100000000000003</v>
       </c>
       <c r="D167" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -3429,13 +3429,13 @@
         <v>1923563</v>
       </c>
       <c r="B168" t="s">
-        <v>121</v>
+        <v>57</v>
       </c>
       <c r="C168">
         <v>0.01</v>
       </c>
       <c r="D168" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -3443,13 +3443,13 @@
         <v>1923562</v>
       </c>
       <c r="B169" t="s">
-        <v>122</v>
+        <v>211</v>
       </c>
       <c r="C169">
         <v>0.01</v>
       </c>
       <c r="D169" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -3457,13 +3457,13 @@
         <v>24556794</v>
       </c>
       <c r="B170" t="s">
-        <v>123</v>
+        <v>212</v>
       </c>
       <c r="C170">
         <v>0.01</v>
       </c>
       <c r="D170" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -3471,13 +3471,13 @@
         <v>24525623</v>
       </c>
       <c r="B171" t="s">
-        <v>124</v>
+        <v>213</v>
       </c>
       <c r="C171">
         <v>0.01</v>
       </c>
       <c r="D171" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -3485,13 +3485,13 @@
         <v>24421186</v>
       </c>
       <c r="B172" t="s">
-        <v>125</v>
+        <v>214</v>
       </c>
       <c r="C172">
         <v>0.01</v>
       </c>
       <c r="D172" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -3499,13 +3499,13 @@
         <v>24421187</v>
       </c>
       <c r="B173" t="s">
-        <v>126</v>
+        <v>215</v>
       </c>
       <c r="C173">
         <v>0.01</v>
       </c>
       <c r="D173" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -3513,13 +3513,13 @@
         <v>24421188</v>
       </c>
       <c r="B174" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="C174">
         <v>0.01</v>
       </c>
       <c r="D174" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -3527,13 +3527,13 @@
         <v>24421189</v>
       </c>
       <c r="B175" t="s">
-        <v>128</v>
+        <v>217</v>
       </c>
       <c r="C175">
         <v>0.01</v>
       </c>
       <c r="D175" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -3541,13 +3541,13 @@
         <v>1238234</v>
       </c>
       <c r="B176" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="C176">
         <v>5.88</v>
       </c>
       <c r="D176" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -3555,13 +3555,13 @@
         <v>1238240</v>
       </c>
       <c r="B177" t="s">
-        <v>174</v>
+        <v>74</v>
       </c>
       <c r="C177">
         <v>5.88</v>
       </c>
       <c r="D177" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -3569,13 +3569,13 @@
         <v>1238241</v>
       </c>
       <c r="B178" t="s">
-        <v>175</v>
+        <v>75</v>
       </c>
       <c r="C178">
         <v>5.88</v>
       </c>
       <c r="D178" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -3583,13 +3583,13 @@
         <v>24479430</v>
       </c>
       <c r="B179" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="C179">
         <v>7.04</v>
       </c>
       <c r="D179" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -3597,13 +3597,13 @@
         <v>24479426</v>
       </c>
       <c r="B180" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="C180">
         <v>7.04</v>
       </c>
       <c r="D180" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -3611,13 +3611,13 @@
         <v>24479425</v>
       </c>
       <c r="B181" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="C181">
         <v>7.04</v>
       </c>
       <c r="D181" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -3625,13 +3625,13 @@
         <v>24479427</v>
       </c>
       <c r="B182" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="C182">
         <v>11.9</v>
       </c>
       <c r="D182" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -3639,13 +3639,13 @@
         <v>24479428</v>
       </c>
       <c r="B183" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="C183">
         <v>9.8000000000000007</v>
       </c>
       <c r="D183" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -3653,13 +3653,13 @@
         <v>24479429</v>
       </c>
       <c r="B184" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="C184">
         <v>10.09</v>
       </c>
       <c r="D184" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -3667,13 +3667,13 @@
         <v>24479431</v>
       </c>
       <c r="B185" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="C185">
         <v>7.04</v>
       </c>
       <c r="D185" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -3681,13 +3681,13 @@
         <v>24479432</v>
       </c>
       <c r="B186" t="s">
-        <v>183</v>
+        <v>152</v>
       </c>
       <c r="C186">
         <v>11.9</v>
       </c>
       <c r="D186" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
@@ -3695,13 +3695,13 @@
         <v>24488138</v>
       </c>
       <c r="B187" t="s">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="C187">
         <v>0.01</v>
       </c>
       <c r="D187" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -3709,13 +3709,13 @@
         <v>579883</v>
       </c>
       <c r="B188" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="C188">
         <v>11.25</v>
       </c>
       <c r="D188" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -3723,13 +3723,13 @@
         <v>809083</v>
       </c>
       <c r="B189" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="C189">
         <v>19.239999999999998</v>
       </c>
       <c r="D189" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -3737,13 +3737,13 @@
         <v>369644</v>
       </c>
       <c r="B190" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C190">
         <v>10.5</v>
       </c>
       <c r="D190" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -3751,13 +3751,13 @@
         <v>378328</v>
       </c>
       <c r="B191" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="C191">
         <v>14.4</v>
       </c>
       <c r="D191" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
@@ -3765,13 +3765,13 @@
         <v>24507775</v>
       </c>
       <c r="B192" t="s">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="C192">
         <v>28.8</v>
       </c>
       <c r="D192" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
@@ -3779,13 +3779,13 @@
         <v>620140</v>
       </c>
       <c r="B193" t="s">
-        <v>134</v>
+        <v>60</v>
       </c>
       <c r="C193">
         <v>147.38999999999999</v>
       </c>
       <c r="D193" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -3793,13 +3793,13 @@
         <v>24507774</v>
       </c>
       <c r="B194" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="C194">
         <v>51.7</v>
       </c>
       <c r="D194" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
@@ -3807,13 +3807,13 @@
         <v>626677</v>
       </c>
       <c r="B195" t="s">
-        <v>136</v>
+        <v>62</v>
       </c>
       <c r="C195">
         <v>20.75</v>
       </c>
       <c r="D195" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -3821,13 +3821,13 @@
         <v>789437</v>
       </c>
       <c r="B196" t="s">
-        <v>137</v>
+        <v>63</v>
       </c>
       <c r="C196">
         <v>5.98</v>
       </c>
       <c r="D196" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
@@ -3835,13 +3835,13 @@
         <v>355534</v>
       </c>
       <c r="B197" t="s">
-        <v>138</v>
+        <v>64</v>
       </c>
       <c r="C197">
         <v>10.1</v>
       </c>
       <c r="D197" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -3849,13 +3849,13 @@
         <v>355535</v>
       </c>
       <c r="B198" t="s">
-        <v>139</v>
+        <v>218</v>
       </c>
       <c r="C198">
         <v>12.9</v>
       </c>
       <c r="D198" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -3863,13 +3863,13 @@
         <v>116457</v>
       </c>
       <c r="B199" t="s">
-        <v>140</v>
+        <v>219</v>
       </c>
       <c r="C199">
         <v>0.01</v>
       </c>
       <c r="D199" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
@@ -3877,13 +3877,13 @@
         <v>24449148</v>
       </c>
       <c r="B200" t="s">
-        <v>141</v>
+        <v>220</v>
       </c>
       <c r="C200">
         <v>3.5</v>
       </c>
       <c r="D200" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -3891,13 +3891,13 @@
         <v>395073</v>
       </c>
       <c r="B201" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C201">
         <v>62.5</v>
       </c>
       <c r="D201" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -3905,13 +3905,13 @@
         <v>2846332</v>
       </c>
       <c r="B202" t="s">
-        <v>143</v>
+        <v>65</v>
       </c>
       <c r="C202">
         <v>0.01</v>
       </c>
       <c r="D202" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
@@ -3919,13 +3919,13 @@
         <v>24307465</v>
       </c>
       <c r="B203" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C203">
         <v>0.01</v>
       </c>
       <c r="D203" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -3933,13 +3933,13 @@
         <v>1897666</v>
       </c>
       <c r="B204" t="s">
-        <v>146</v>
+        <v>67</v>
       </c>
       <c r="C204">
         <v>1.77</v>
       </c>
       <c r="D204" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
@@ -3947,13 +3947,13 @@
         <v>1897667</v>
       </c>
       <c r="B205" t="s">
-        <v>147</v>
+        <v>221</v>
       </c>
       <c r="C205">
         <v>0.4</v>
       </c>
       <c r="D205" t="s">
-        <v>116</v>
+        <v>54</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
@@ -3961,13 +3961,13 @@
         <v>732290</v>
       </c>
       <c r="B206" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="C206">
         <v>6.08</v>
       </c>
       <c r="D206" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved the routes for items into the routes folder, everthing is in place in order to start building the front end and connecting it to the back end.
</commit_message>
<xml_diff>
--- a/server/db/supplies_book_1.xlsx
+++ b/server/db/supplies_book_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorvil/Desktop/STEVEN(hard drive)/EDUCATION/CUNY SPS - BS Information Systems/2023 FALL/IS 499/classwork/staples-supply-management/server/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B26527-186B-5743-BF04-B28423CFDF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6B7C50-3C73-5A49-A99D-933C5773A716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1840" windowWidth="21600" windowHeight="16160" xr2:uid="{19EE4B8A-1A9E-42DD-BAFB-81936C1DA736}"/>
   </bookViews>
@@ -1075,7 +1075,7 @@
   <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>